<commit_message>
Sat Aug 23 13:11:49 EDT 2025
</commit_message>
<xml_diff>
--- a/Doont.xlsx
+++ b/Doont.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cmatt\OneDrive\_Doont\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cmatt\OneDrive\doont\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4CEA9897-CE58-4251-81C1-F48647D0A363}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77629057-8B50-4324-AC8C-95A41A6EB31A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3240" yWindow="960" windowWidth="15945" windowHeight="11880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3630" yWindow="1290" windowWidth="19815" windowHeight="11880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Game_Record" sheetId="1" r:id="rId1"/>
@@ -171,7 +171,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -181,6 +181,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="1" tint="4.9989318521683403E-2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -259,10 +265,10 @@
     <xf numFmtId="164" fontId="4" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -548,7 +554,7 @@
   <dimension ref="A1:H8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+      <selection activeCell="H4" sqref="H4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -583,7 +589,7 @@
       <c r="F1" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="16"/>
+      <c r="G1" s="17"/>
       <c r="H1" s="14" t="s">
         <v>22</v>
       </c>
@@ -608,7 +614,7 @@
       <c r="F2" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="H2" s="17">
+      <c r="H2" s="16">
         <f>COUNTA(Game_Record!B2:B100)</f>
         <v>7</v>
       </c>
@@ -748,7 +754,7 @@
   <dimension ref="A1:K9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="L1" sqref="L1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Sun Aug 24 02:29:31 EDT 2025
</commit_message>
<xml_diff>
--- a/Doont.xlsx
+++ b/Doont.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cmatt\OneDrive\doont\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77629057-8B50-4324-AC8C-95A41A6EB31A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E6349A8-3E06-46D0-8440-C349F1840EF1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3630" yWindow="1290" windowWidth="19815" windowHeight="11880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Game_Record" sheetId="1" r:id="rId1"/>
@@ -37,26 +37,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="23">
-  <si>
-    <t>Game #</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="19">
   <si>
     <t>Date</t>
   </si>
   <si>
-    <t>1st Place</t>
-  </si>
-  <si>
-    <t>2nd Place</t>
-  </si>
-  <si>
-    <t>3rd Place</t>
-  </si>
-  <si>
-    <t>4th Place</t>
-  </si>
-  <si>
     <t>Player</t>
   </si>
   <si>
@@ -106,6 +91,9 @@
   </si>
   <si>
     <t>Total Games Played</t>
+  </si>
+  <si>
+    <t>Game</t>
   </si>
 </sst>
 </file>
@@ -115,7 +103,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd;@"/>
   </numFmts>
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -156,13 +144,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="14"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="16"/>
       <color theme="1"/>
@@ -171,7 +152,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -181,12 +162,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="1" tint="4.9989318521683403E-2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -218,7 +193,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -265,10 +240,7 @@
     <xf numFmtId="164" fontId="4" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -551,10 +523,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H8"/>
+  <dimension ref="A1:F8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H4" sqref="H4"/>
+      <selection activeCell="J9" sqref="J9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -565,36 +537,30 @@
     <col min="4" max="4" width="14.7109375" style="5" customWidth="1"/>
     <col min="5" max="5" width="16.140625" style="5" customWidth="1"/>
     <col min="6" max="6" width="17.42578125" style="5" customWidth="1"/>
-    <col min="7" max="7" width="9.140625" style="5"/>
-    <col min="8" max="8" width="25.5703125" style="5" customWidth="1"/>
-    <col min="9" max="16384" width="9.140625" style="5"/>
+    <col min="7" max="16384" width="9.140625" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A1" s="14" t="s">
-        <v>0</v>
+        <v>18</v>
       </c>
       <c r="B1" s="15" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C1" s="14" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D1" s="14" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E1" s="14" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="F1" s="14" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" s="17"/>
-      <c r="H1" s="14" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" ht="21" x14ac:dyDescent="0.25">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
         <f>ROW()-1</f>
         <v>1</v>
@@ -603,23 +569,19 @@
         <v>45865</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="H2" s="16">
-        <f>COUNTA(Game_Record!B2:B100)</f>
-        <v>7</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
         <f t="shared" ref="A3:A7" si="0">ROW()-1</f>
         <v>2</v>
@@ -628,19 +590,19 @@
         <v>45872</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
         <f t="shared" si="0"/>
         <v>3</v>
@@ -649,19 +611,19 @@
         <v>45876</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
         <f t="shared" si="0"/>
         <v>4</v>
@@ -670,19 +632,19 @@
         <v>45879</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="E5" s="5" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="F5" s="5" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
         <f t="shared" si="0"/>
         <v>5</v>
@@ -691,19 +653,19 @@
         <v>45883</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
         <f t="shared" si="0"/>
         <v>6</v>
@@ -712,19 +674,19 @@
         <v>45888</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="D7" s="5" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="5">
         <v>7</v>
       </c>
@@ -732,16 +694,16 @@
         <v>45890</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="D8" s="5" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="E8" s="5" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
     </row>
   </sheetData>
@@ -751,10 +713,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E6444F9B-2DCC-4DAB-89DA-045932047514}">
-  <dimension ref="A1:K9"/>
+  <dimension ref="A1:L9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="L1" sqref="L1"/>
+      <selection activeCell="L2" sqref="L2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -769,66 +731,70 @@
     <col min="9" max="9" width="20.28515625" style="5" customWidth="1"/>
     <col min="10" max="10" width="18" style="11" customWidth="1"/>
     <col min="11" max="11" width="13.28515625" style="5" customWidth="1"/>
-    <col min="12" max="16384" width="9.140625" style="5"/>
+    <col min="12" max="12" width="28.5703125" style="5" customWidth="1"/>
+    <col min="13" max="16384" width="9.140625" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="37.5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" ht="56.25" x14ac:dyDescent="0.25">
       <c r="A1" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="E1" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="F1" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="B1" s="12" t="s">
+      <c r="G1" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="H1" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="I1" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="J1" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="K1" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="C1" s="12" t="s">
-        <v>8</v>
-      </c>
-      <c r="D1" s="12" t="s">
-        <v>9</v>
-      </c>
-      <c r="E1" s="12" t="s">
+      <c r="L1" s="14" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" ht="21" x14ac:dyDescent="0.25">
+      <c r="A2" s="9" t="s">
         <v>10</v>
-      </c>
-      <c r="F1" s="12" t="s">
-        <v>11</v>
-      </c>
-      <c r="G1" s="12" t="s">
-        <v>14</v>
-      </c>
-      <c r="H1" s="12" t="s">
-        <v>20</v>
-      </c>
-      <c r="I1" s="12" t="s">
-        <v>21</v>
-      </c>
-      <c r="J1" s="13" t="s">
-        <v>13</v>
-      </c>
-      <c r="K1" s="12" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A2" s="9" t="s">
-        <v>15</v>
       </c>
       <c r="B2" s="2">
         <f xml:space="preserve"> C2 + D2 + E2 + F2</f>
         <v>5</v>
       </c>
       <c r="C2" s="2">
-        <f>COUNTIF(Game_Record!C2:C100, "Doanage")</f>
+        <f>COUNTIF(Game_Record!C2:C74, "Doanage")</f>
         <v>4</v>
       </c>
       <c r="D2" s="2">
-        <f>COUNTIF(Game_Record!D2:D100, "Doanage")</f>
+        <f>COUNTIF(Game_Record!D2:D74, "Doanage")</f>
         <v>1</v>
       </c>
       <c r="E2" s="2">
-        <f>COUNTIF(Game_Record!E2:E100, "Doanage")</f>
+        <f>COUNTIF(Game_Record!E2:E74, "Doanage")</f>
         <v>0</v>
       </c>
       <c r="F2" s="2">
-        <f>COUNTIF(Game_Record!F2:F100, "Doanage")</f>
+        <f>COUNTIF(Game_Record!F2:F74, "Doanage")</f>
         <v>0</v>
       </c>
       <c r="G2" s="3">
@@ -839,9 +805,9 @@
         <f xml:space="preserve"> (C2+D2) / B2</f>
         <v>1</v>
       </c>
-      <c r="I2" s="7">
-        <f xml:space="preserve"> B2 / Game_Record!$H$2</f>
-        <v>0.7142857142857143</v>
+      <c r="I2" s="7" t="e">
+        <f xml:space="preserve"> B2 / Game_Record!#REF!</f>
+        <v>#REF!</v>
       </c>
       <c r="J2" s="10">
         <f xml:space="preserve"> K2/B2</f>
@@ -851,29 +817,33 @@
         <f xml:space="preserve"> (C2 * 5) + (D2 * 3) + (E2 * 1)</f>
         <v>23</v>
       </c>
-    </row>
-    <row r="3" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="L2" s="16">
+        <f>COUNTA(Game_Record!B2:B100)</f>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" s="9" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="B3" s="2">
         <f xml:space="preserve"> C3 + D3 + E3 + F3</f>
         <v>5</v>
       </c>
       <c r="C3" s="2">
-        <f>COUNTIF(Game_Record!C2:C100, "SiderFace")</f>
+        <f>COUNTIF(Game_Record!C2:C74, "SiderFace")</f>
         <v>1</v>
       </c>
       <c r="D3" s="2">
-        <f>COUNTIF(Game_Record!D2:D100, "SiderFace")</f>
+        <f>COUNTIF(Game_Record!D2:D74, "SiderFace")</f>
         <v>4</v>
       </c>
       <c r="E3" s="2">
-        <f>COUNTIF(Game_Record!E2:E100, "SiderFace")</f>
+        <f>COUNTIF(Game_Record!E2:E74, "SiderFace")</f>
         <v>0</v>
       </c>
       <c r="F3" s="2">
-        <f>COUNTIF(Game_Record!F2:F100, "SiderFace")</f>
+        <f>COUNTIF(Game_Record!F2:F74, "SiderFace")</f>
         <v>0</v>
       </c>
       <c r="G3" s="3">
@@ -884,9 +854,9 @@
         <f xml:space="preserve"> (C3+D3) / B3</f>
         <v>1</v>
       </c>
-      <c r="I3" s="7">
-        <f xml:space="preserve"> B3 / Game_Record!$H$2</f>
-        <v>0.7142857142857143</v>
+      <c r="I3" s="7" t="e">
+        <f xml:space="preserve"> B3 / Game_Record!#REF!</f>
+        <v>#REF!</v>
       </c>
       <c r="J3" s="10">
         <f xml:space="preserve"> K3/B3</f>
@@ -897,28 +867,28 @@
         <v>17</v>
       </c>
     </row>
-    <row r="4" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A4" s="9" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="B4" s="2">
         <f xml:space="preserve"> C4 + D4 + E4 + F4</f>
         <v>6</v>
       </c>
       <c r="C4" s="2">
-        <f>COUNTIF(Game_Record!C2:C100, "DrSystomatix")</f>
+        <f>COUNTIF(Game_Record!C2:C74, "DrSystomatix")</f>
         <v>0</v>
       </c>
       <c r="D4" s="2">
-        <f>COUNTIF(Game_Record!D2:D100, "DrSystomatix")</f>
+        <f>COUNTIF(Game_Record!D2:D74, "DrSystomatix")</f>
         <v>1</v>
       </c>
       <c r="E4" s="2">
-        <f>COUNTIF(Game_Record!E2:E100, "DrSystomatix")</f>
+        <f>COUNTIF(Game_Record!E2:E74, "DrSystomatix")</f>
         <v>3</v>
       </c>
       <c r="F4" s="2">
-        <f>COUNTIF(Game_Record!F2:F100, "DrSystomatix")</f>
+        <f>COUNTIF(Game_Record!F2:F74, "DrSystomatix")</f>
         <v>2</v>
       </c>
       <c r="G4" s="3">
@@ -929,9 +899,9 @@
         <f xml:space="preserve"> (C4+D4) / B4</f>
         <v>0.16666666666666666</v>
       </c>
-      <c r="I4" s="7">
-        <f xml:space="preserve"> B4 / Game_Record!$H$2</f>
-        <v>0.8571428571428571</v>
+      <c r="I4" s="7" t="e">
+        <f xml:space="preserve"> B4 / Game_Record!#REF!</f>
+        <v>#REF!</v>
       </c>
       <c r="J4" s="10">
         <f xml:space="preserve"> K4/B4</f>
@@ -942,28 +912,28 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A5" s="9" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="B5" s="2">
         <f xml:space="preserve"> C5 + D5 + E5 + F5</f>
         <v>6</v>
       </c>
       <c r="C5" s="2">
-        <f>COUNTIF(Game_Record!C2:C100, "Player1")</f>
+        <f>COUNTIF(Game_Record!C2:C74, "Player1")</f>
         <v>2</v>
       </c>
       <c r="D5" s="2">
-        <f>COUNTIF(Game_Record!D2:D100, "Player1")</f>
+        <f>COUNTIF(Game_Record!D2:D74, "Player1")</f>
         <v>1</v>
       </c>
       <c r="E5" s="2">
-        <f>COUNTIF(Game_Record!E2:E100, "Player1")</f>
+        <f>COUNTIF(Game_Record!E2:E74, "Player1")</f>
         <v>3</v>
       </c>
       <c r="F5" s="2">
-        <f>COUNTIF(Game_Record!F2:F100, "Player1")</f>
+        <f>COUNTIF(Game_Record!F2:F74, "Player1")</f>
         <v>0</v>
       </c>
       <c r="G5" s="3">
@@ -974,9 +944,9 @@
         <f xml:space="preserve"> (C5+D5) / B5</f>
         <v>0.5</v>
       </c>
-      <c r="I5" s="7">
-        <f xml:space="preserve"> B5 / Game_Record!$H$2</f>
-        <v>0.8571428571428571</v>
+      <c r="I5" s="7" t="e">
+        <f xml:space="preserve"> B5 / Game_Record!#REF!</f>
+        <v>#REF!</v>
       </c>
       <c r="J5" s="10">
         <f xml:space="preserve"> K5/B5</f>
@@ -987,28 +957,28 @@
         <v>16</v>
       </c>
     </row>
-    <row r="6" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A6" s="9" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="B6" s="2">
         <f xml:space="preserve"> C6 + D6 + E6 + F6</f>
         <v>6</v>
       </c>
       <c r="C6" s="2">
-        <f>COUNTIF(Game_Record!C2:C100, "SimpleJack")</f>
+        <f>COUNTIF(Game_Record!C2:C74, "SimpleJack")</f>
         <v>0</v>
       </c>
       <c r="D6" s="2">
-        <f>COUNTIF(Game_Record!D2:D100, "SimpleJack")</f>
+        <f>COUNTIF(Game_Record!D2:D74, "SimpleJack")</f>
         <v>0</v>
       </c>
       <c r="E6" s="2">
-        <f>COUNTIF(Game_Record!E2:E100, "SimpleJack")</f>
+        <f>COUNTIF(Game_Record!E2:E74, "SimpleJack")</f>
         <v>1</v>
       </c>
       <c r="F6" s="2">
-        <f>COUNTIF(Game_Record!F2:F100, "SimpleJack")</f>
+        <f>COUNTIF(Game_Record!F2:F74, "SimpleJack")</f>
         <v>5</v>
       </c>
       <c r="G6" s="3">
@@ -1019,9 +989,9 @@
         <f xml:space="preserve"> (C6+D6) / B6</f>
         <v>0</v>
       </c>
-      <c r="I6" s="7">
-        <f xml:space="preserve"> B6 / Game_Record!$H$2</f>
-        <v>0.8571428571428571</v>
+      <c r="I6" s="7" t="e">
+        <f xml:space="preserve"> B6 / Game_Record!#REF!</f>
+        <v>#REF!</v>
       </c>
       <c r="J6" s="10">
         <f xml:space="preserve"> K6/B6</f>
@@ -1032,7 +1002,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" s="1"/>
       <c r="B9" s="8"/>
     </row>

</xml_diff>

<commit_message>
Thu, Sep  4, 2025  2:59:24 PM
</commit_message>
<xml_diff>
--- a/Doont.xlsx
+++ b/Doont.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cmatt\OneDrive\doont\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cmatt\OneDrive\_Doont\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E6349A8-3E06-46D0-8440-C349F1840EF1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DAA8605B-D9B3-4D9B-BF60-97807A2E23BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="31965" yWindow="2385" windowWidth="19815" windowHeight="11880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Game_Record" sheetId="1" r:id="rId1"/>
@@ -37,11 +37,26 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="23">
+  <si>
+    <t>Game #</t>
+  </si>
   <si>
     <t>Date</t>
   </si>
   <si>
+    <t>1st Place</t>
+  </si>
+  <si>
+    <t>2nd Place</t>
+  </si>
+  <si>
+    <t>3rd Place</t>
+  </si>
+  <si>
+    <t>4th Place</t>
+  </si>
+  <si>
     <t>Player</t>
   </si>
   <si>
@@ -91,9 +106,6 @@
   </si>
   <si>
     <t>Total Games Played</t>
-  </si>
-  <si>
-    <t>Game</t>
   </si>
 </sst>
 </file>
@@ -103,7 +115,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd;@"/>
   </numFmts>
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -137,6 +149,13 @@
     </font>
     <font>
       <b/>
+      <sz val="14"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="14"/>
       <color theme="0"/>
       <name val="Calibri"/>
@@ -193,7 +212,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -240,7 +259,10 @@
     <xf numFmtId="164" fontId="4" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -523,10 +545,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F8"/>
+  <dimension ref="A1:H10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J9" sqref="J9"/>
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -537,30 +559,36 @@
     <col min="4" max="4" width="14.7109375" style="5" customWidth="1"/>
     <col min="5" max="5" width="16.140625" style="5" customWidth="1"/>
     <col min="6" max="6" width="17.42578125" style="5" customWidth="1"/>
-    <col min="7" max="16384" width="9.140625" style="5"/>
+    <col min="7" max="7" width="9.140625" style="5"/>
+    <col min="8" max="8" width="25.5703125" style="5" customWidth="1"/>
+    <col min="9" max="16384" width="9.140625" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A1" s="14" t="s">
-        <v>18</v>
+        <v>0</v>
       </c>
       <c r="B1" s="15" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C1" s="14" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="D1" s="14" t="s">
+      <c r="E1" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="E1" s="14" t="s">
+      <c r="F1" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="F1" s="14" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G1" s="16"/>
+      <c r="H1" s="14" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" ht="21" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
         <f>ROW()-1</f>
         <v>1</v>
@@ -569,19 +597,23 @@
         <v>45865</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+        <v>18</v>
+      </c>
+      <c r="H2" s="17">
+        <f>COUNTA(Game_Record!B2:B100)</f>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
         <f t="shared" ref="A3:A7" si="0">ROW()-1</f>
         <v>2</v>
@@ -590,19 +622,19 @@
         <v>45872</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
         <f t="shared" si="0"/>
         <v>3</v>
@@ -611,19 +643,19 @@
         <v>45876</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
         <f t="shared" si="0"/>
         <v>4</v>
@@ -632,19 +664,19 @@
         <v>45879</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="E5" s="5" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="F5" s="5" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
         <f t="shared" si="0"/>
         <v>5</v>
@@ -653,19 +685,19 @@
         <v>45883</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
         <f t="shared" si="0"/>
         <v>6</v>
@@ -674,36 +706,79 @@
         <v>45888</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="D7" s="5" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="5">
+        <f>ROW()-1</f>
         <v>7</v>
       </c>
       <c r="B8" s="6">
         <v>45890</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="D8" s="5" t="s">
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="E8" s="5" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>13</v>
+        <v>18</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A9" s="5">
+        <f>ROW()-1</f>
+        <v>8</v>
+      </c>
+      <c r="B9" s="6">
+        <v>45899</v>
+      </c>
+      <c r="C9" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="D9" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="E9" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="F9" s="5" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A10" s="5">
+        <f>ROW()-1</f>
+        <v>9</v>
+      </c>
+      <c r="B10" s="6">
+        <v>45901</v>
+      </c>
+      <c r="C10" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="D10" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="E10" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="F10" s="5" t="s">
+        <v>19</v>
       </c>
     </row>
   </sheetData>
@@ -713,10 +788,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E6444F9B-2DCC-4DAB-89DA-045932047514}">
-  <dimension ref="A1:L9"/>
+  <dimension ref="A1:K9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="L2" sqref="L2"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -731,119 +806,111 @@
     <col min="9" max="9" width="20.28515625" style="5" customWidth="1"/>
     <col min="10" max="10" width="18" style="11" customWidth="1"/>
     <col min="11" max="11" width="13.28515625" style="5" customWidth="1"/>
-    <col min="12" max="12" width="28.5703125" style="5" customWidth="1"/>
-    <col min="13" max="16384" width="9.140625" style="5"/>
+    <col min="12" max="16384" width="9.140625" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="56.25" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" ht="37.5" x14ac:dyDescent="0.25">
       <c r="A1" s="12" t="s">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="B1" s="12" t="s">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="C1" s="12" t="s">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="D1" s="12" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="E1" s="12" t="s">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="F1" s="12" t="s">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="G1" s="12" t="s">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="H1" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="I1" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="J1" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="K1" s="12" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A2" s="9" t="s">
         <v>15</v>
-      </c>
-      <c r="I1" s="12" t="s">
-        <v>16</v>
-      </c>
-      <c r="J1" s="13" t="s">
-        <v>8</v>
-      </c>
-      <c r="K1" s="12" t="s">
-        <v>7</v>
-      </c>
-      <c r="L1" s="14" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="2" spans="1:12" ht="21" x14ac:dyDescent="0.25">
-      <c r="A2" s="9" t="s">
-        <v>10</v>
       </c>
       <c r="B2" s="2">
         <f xml:space="preserve"> C2 + D2 + E2 + F2</f>
+        <v>7</v>
+      </c>
+      <c r="C2" s="2">
+        <f>COUNTIF(Game_Record!C2:C100, "Doanage")</f>
         <v>5</v>
       </c>
-      <c r="C2" s="2">
-        <f>COUNTIF(Game_Record!C2:C74, "Doanage")</f>
-        <v>4</v>
-      </c>
       <c r="D2" s="2">
-        <f>COUNTIF(Game_Record!D2:D74, "Doanage")</f>
-        <v>1</v>
+        <f>COUNTIF(Game_Record!D2:D100, "Doanage")</f>
+        <v>2</v>
       </c>
       <c r="E2" s="2">
-        <f>COUNTIF(Game_Record!E2:E74, "Doanage")</f>
+        <f>COUNTIF(Game_Record!E2:E100, "Doanage")</f>
         <v>0</v>
       </c>
       <c r="F2" s="2">
-        <f>COUNTIF(Game_Record!F2:F74, "Doanage")</f>
+        <f>COUNTIF(Game_Record!F2:F100, "Doanage")</f>
         <v>0</v>
       </c>
       <c r="G2" s="3">
         <f xml:space="preserve"> C2 / B2</f>
-        <v>0.8</v>
+        <v>0.7142857142857143</v>
       </c>
       <c r="H2" s="7">
         <f xml:space="preserve"> (C2+D2) / B2</f>
         <v>1</v>
       </c>
-      <c r="I2" s="7" t="e">
-        <f xml:space="preserve"> B2 / Game_Record!#REF!</f>
-        <v>#REF!</v>
+      <c r="I2" s="7">
+        <f xml:space="preserve"> B2 / Game_Record!$H$2</f>
+        <v>0.77777777777777779</v>
       </c>
       <c r="J2" s="10">
         <f xml:space="preserve"> K2/B2</f>
-        <v>4.5999999999999996</v>
+        <v>4.4285714285714288</v>
       </c>
       <c r="K2" s="2">
         <f xml:space="preserve"> (C2 * 5) + (D2 * 3) + (E2 * 1)</f>
-        <v>23</v>
-      </c>
-      <c r="L2" s="16">
-        <f>COUNTA(Game_Record!B2:B100)</f>
-        <v>7</v>
-      </c>
-    </row>
-    <row r="3" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" s="9" t="s">
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="B3" s="2">
         <f xml:space="preserve"> C3 + D3 + E3 + F3</f>
         <v>5</v>
       </c>
       <c r="C3" s="2">
-        <f>COUNTIF(Game_Record!C2:C74, "SiderFace")</f>
+        <f>COUNTIF(Game_Record!C2:C100, "SiderFace")</f>
         <v>1</v>
       </c>
       <c r="D3" s="2">
-        <f>COUNTIF(Game_Record!D2:D74, "SiderFace")</f>
+        <f>COUNTIF(Game_Record!D2:D100, "SiderFace")</f>
         <v>4</v>
       </c>
       <c r="E3" s="2">
-        <f>COUNTIF(Game_Record!E2:E74, "SiderFace")</f>
+        <f>COUNTIF(Game_Record!E2:E100, "SiderFace")</f>
         <v>0</v>
       </c>
       <c r="F3" s="2">
-        <f>COUNTIF(Game_Record!F2:F74, "SiderFace")</f>
+        <f>COUNTIF(Game_Record!F2:F100, "SiderFace")</f>
         <v>0</v>
       </c>
       <c r="G3" s="3">
@@ -854,9 +921,9 @@
         <f xml:space="preserve"> (C3+D3) / B3</f>
         <v>1</v>
       </c>
-      <c r="I3" s="7" t="e">
-        <f xml:space="preserve"> B3 / Game_Record!#REF!</f>
-        <v>#REF!</v>
+      <c r="I3" s="7">
+        <f xml:space="preserve"> B3 / Game_Record!$H$2</f>
+        <v>0.55555555555555558</v>
       </c>
       <c r="J3" s="10">
         <f xml:space="preserve"> K3/B3</f>
@@ -867,29 +934,29 @@
         <v>17</v>
       </c>
     </row>
-    <row r="4" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A4" s="9" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="B4" s="2">
         <f xml:space="preserve"> C4 + D4 + E4 + F4</f>
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="C4" s="2">
-        <f>COUNTIF(Game_Record!C2:C74, "DrSystomatix")</f>
+        <f>COUNTIF(Game_Record!C2:C100, "DrSystomatix")</f>
         <v>0</v>
       </c>
       <c r="D4" s="2">
-        <f>COUNTIF(Game_Record!D2:D74, "DrSystomatix")</f>
+        <f>COUNTIF(Game_Record!D2:D100, "DrSystomatix")</f>
         <v>1</v>
       </c>
       <c r="E4" s="2">
-        <f>COUNTIF(Game_Record!E2:E74, "DrSystomatix")</f>
+        <f>COUNTIF(Game_Record!E2:E100, "DrSystomatix")</f>
         <v>3</v>
       </c>
       <c r="F4" s="2">
-        <f>COUNTIF(Game_Record!F2:F74, "DrSystomatix")</f>
-        <v>2</v>
+        <f>COUNTIF(Game_Record!F2:F100, "DrSystomatix")</f>
+        <v>4</v>
       </c>
       <c r="G4" s="3">
         <f xml:space="preserve"> C4 / B4</f>
@@ -897,88 +964,88 @@
       </c>
       <c r="H4" s="7">
         <f xml:space="preserve"> (C4+D4) / B4</f>
-        <v>0.16666666666666666</v>
-      </c>
-      <c r="I4" s="7" t="e">
-        <f xml:space="preserve"> B4 / Game_Record!#REF!</f>
-        <v>#REF!</v>
+        <v>0.125</v>
+      </c>
+      <c r="I4" s="7">
+        <f xml:space="preserve"> B4 / Game_Record!$H$2</f>
+        <v>0.88888888888888884</v>
       </c>
       <c r="J4" s="10">
         <f xml:space="preserve"> K4/B4</f>
-        <v>1</v>
+        <v>0.75</v>
       </c>
       <c r="K4" s="2">
         <f xml:space="preserve"> (C4 * 5) + (D4 * 3) + (E4 * 1)</f>
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A5" s="9" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="B5" s="2">
         <f xml:space="preserve"> C5 + D5 + E5 + F5</f>
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="C5" s="2">
-        <f>COUNTIF(Game_Record!C2:C74, "Player1")</f>
+        <f>COUNTIF(Game_Record!C2:C100, "Player1")</f>
+        <v>3</v>
+      </c>
+      <c r="D5" s="2">
+        <f>COUNTIF(Game_Record!D2:D100, "Player1")</f>
         <v>2</v>
       </c>
-      <c r="D5" s="2">
-        <f>COUNTIF(Game_Record!D2:D74, "Player1")</f>
-        <v>1</v>
-      </c>
       <c r="E5" s="2">
-        <f>COUNTIF(Game_Record!E2:E74, "Player1")</f>
+        <f>COUNTIF(Game_Record!E2:E100, "Player1")</f>
         <v>3</v>
       </c>
       <c r="F5" s="2">
-        <f>COUNTIF(Game_Record!F2:F74, "Player1")</f>
+        <f>COUNTIF(Game_Record!F2:F100, "Player1")</f>
         <v>0</v>
       </c>
       <c r="G5" s="3">
         <f xml:space="preserve"> C5 / B5</f>
-        <v>0.33333333333333331</v>
+        <v>0.375</v>
       </c>
       <c r="H5" s="7">
         <f xml:space="preserve"> (C5+D5) / B5</f>
-        <v>0.5</v>
-      </c>
-      <c r="I5" s="7" t="e">
-        <f xml:space="preserve"> B5 / Game_Record!#REF!</f>
-        <v>#REF!</v>
+        <v>0.625</v>
+      </c>
+      <c r="I5" s="7">
+        <f xml:space="preserve"> B5 / Game_Record!$H$2</f>
+        <v>0.88888888888888884</v>
       </c>
       <c r="J5" s="10">
         <f xml:space="preserve"> K5/B5</f>
-        <v>2.6666666666666665</v>
+        <v>3</v>
       </c>
       <c r="K5" s="2">
         <f xml:space="preserve"> (C5 * 5) + (D5 * 3) + (E5 * 1)</f>
-        <v>16</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A6" s="9" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="B6" s="2">
         <f xml:space="preserve"> C6 + D6 + E6 + F6</f>
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="C6" s="2">
-        <f>COUNTIF(Game_Record!C2:C74, "SimpleJack")</f>
+        <f>COUNTIF(Game_Record!C2:C100, "SimpleJack")</f>
         <v>0</v>
       </c>
       <c r="D6" s="2">
-        <f>COUNTIF(Game_Record!D2:D74, "SimpleJack")</f>
+        <f>COUNTIF(Game_Record!D2:D100, "SimpleJack")</f>
         <v>0</v>
       </c>
       <c r="E6" s="2">
-        <f>COUNTIF(Game_Record!E2:E74, "SimpleJack")</f>
-        <v>1</v>
+        <f>COUNTIF(Game_Record!E2:E100, "SimpleJack")</f>
+        <v>3</v>
       </c>
       <c r="F6" s="2">
-        <f>COUNTIF(Game_Record!F2:F74, "SimpleJack")</f>
+        <f>COUNTIF(Game_Record!F2:F100, "SimpleJack")</f>
         <v>5</v>
       </c>
       <c r="G6" s="3">
@@ -989,20 +1056,20 @@
         <f xml:space="preserve"> (C6+D6) / B6</f>
         <v>0</v>
       </c>
-      <c r="I6" s="7" t="e">
-        <f xml:space="preserve"> B6 / Game_Record!#REF!</f>
-        <v>#REF!</v>
+      <c r="I6" s="7">
+        <f xml:space="preserve"> B6 / Game_Record!$H$2</f>
+        <v>0.88888888888888884</v>
       </c>
       <c r="J6" s="10">
         <f xml:space="preserve"> K6/B6</f>
-        <v>0.16666666666666666</v>
+        <v>0.375</v>
       </c>
       <c r="K6" s="2">
         <f xml:space="preserve"> (C6 * 5) + (D6 * 3) + (E6 * 1)</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" s="1"/>
       <c r="B9" s="8"/>
     </row>

</xml_diff>

<commit_message>
Sat, Sep  6, 2025  6:44:29 PM
</commit_message>
<xml_diff>
--- a/Doont.xlsx
+++ b/Doont.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cmatt\OneDrive\_Doont\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/c92a8a49db0a351e/doont/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DAA8605B-D9B3-4D9B-BF60-97807A2E23BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="6" documentId="13_ncr:1_{DAA8605B-D9B3-4D9B-BF60-97807A2E23BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B9A290E8-24EE-44DA-B239-011F1CA2090D}"/>
   <bookViews>
-    <workbookView xWindow="31965" yWindow="2385" windowWidth="19815" windowHeight="11880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1950" yWindow="1950" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Game_Record" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="23">
   <si>
     <t>Game #</t>
   </si>
@@ -545,10 +545,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H10"/>
+  <dimension ref="A1:H11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+      <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -610,7 +610,7 @@
       </c>
       <c r="H2" s="17">
         <f>COUNTA(Game_Record!B2:B100)</f>
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
@@ -779,6 +779,27 @@
       </c>
       <c r="F10" s="5" t="s">
         <v>19</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A11" s="5">
+        <f>ROW()-1</f>
+        <v>10</v>
+      </c>
+      <c r="B11" s="6">
+        <v>45906</v>
+      </c>
+      <c r="C11" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="D11" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="E11" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="F11" s="5" t="s">
+        <v>18</v>
       </c>
     </row>
   </sheetData>
@@ -850,11 +871,11 @@
       </c>
       <c r="B2" s="2">
         <f xml:space="preserve"> C2 + D2 + E2 + F2</f>
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C2" s="2">
         <f>COUNTIF(Game_Record!C2:C100, "Doanage")</f>
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D2" s="2">
         <f>COUNTIF(Game_Record!D2:D100, "Doanage")</f>
@@ -870,7 +891,7 @@
       </c>
       <c r="G2" s="3">
         <f xml:space="preserve"> C2 / B2</f>
-        <v>0.7142857142857143</v>
+        <v>0.75</v>
       </c>
       <c r="H2" s="7">
         <f xml:space="preserve"> (C2+D2) / B2</f>
@@ -878,15 +899,15 @@
       </c>
       <c r="I2" s="7">
         <f xml:space="preserve"> B2 / Game_Record!$H$2</f>
-        <v>0.77777777777777779</v>
+        <v>0.8</v>
       </c>
       <c r="J2" s="10">
         <f xml:space="preserve"> K2/B2</f>
-        <v>4.4285714285714288</v>
+        <v>4.5</v>
       </c>
       <c r="K2" s="2">
         <f xml:space="preserve"> (C2 * 5) + (D2 * 3) + (E2 * 1)</f>
-        <v>31</v>
+        <v>36</v>
       </c>
     </row>
     <row r="3" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
@@ -895,7 +916,7 @@
       </c>
       <c r="B3" s="2">
         <f xml:space="preserve"> C3 + D3 + E3 + F3</f>
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C3" s="2">
         <f>COUNTIF(Game_Record!C2:C100, "SiderFace")</f>
@@ -903,7 +924,7 @@
       </c>
       <c r="D3" s="2">
         <f>COUNTIF(Game_Record!D2:D100, "SiderFace")</f>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="E3" s="2">
         <f>COUNTIF(Game_Record!E2:E100, "SiderFace")</f>
@@ -915,7 +936,7 @@
       </c>
       <c r="G3" s="3">
         <f xml:space="preserve"> C3 / B3</f>
-        <v>0.2</v>
+        <v>0.16666666666666666</v>
       </c>
       <c r="H3" s="7">
         <f xml:space="preserve"> (C3+D3) / B3</f>
@@ -923,15 +944,15 @@
       </c>
       <c r="I3" s="7">
         <f xml:space="preserve"> B3 / Game_Record!$H$2</f>
-        <v>0.55555555555555558</v>
+        <v>0.6</v>
       </c>
       <c r="J3" s="10">
         <f xml:space="preserve"> K3/B3</f>
-        <v>3.4</v>
+        <v>3.3333333333333335</v>
       </c>
       <c r="K3" s="2">
         <f xml:space="preserve"> (C3 * 5) + (D3 * 3) + (E3 * 1)</f>
-        <v>17</v>
+        <v>20</v>
       </c>
     </row>
     <row r="4" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
@@ -968,7 +989,7 @@
       </c>
       <c r="I4" s="7">
         <f xml:space="preserve"> B4 / Game_Record!$H$2</f>
-        <v>0.88888888888888884</v>
+        <v>0.8</v>
       </c>
       <c r="J4" s="10">
         <f xml:space="preserve"> K4/B4</f>
@@ -985,7 +1006,7 @@
       </c>
       <c r="B5" s="2">
         <f xml:space="preserve"> C5 + D5 + E5 + F5</f>
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C5" s="2">
         <f>COUNTIF(Game_Record!C2:C100, "Player1")</f>
@@ -997,7 +1018,7 @@
       </c>
       <c r="E5" s="2">
         <f>COUNTIF(Game_Record!E2:E100, "Player1")</f>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F5" s="2">
         <f>COUNTIF(Game_Record!F2:F100, "Player1")</f>
@@ -1005,23 +1026,23 @@
       </c>
       <c r="G5" s="3">
         <f xml:space="preserve"> C5 / B5</f>
-        <v>0.375</v>
+        <v>0.33333333333333331</v>
       </c>
       <c r="H5" s="7">
         <f xml:space="preserve"> (C5+D5) / B5</f>
-        <v>0.625</v>
+        <v>0.55555555555555558</v>
       </c>
       <c r="I5" s="7">
         <f xml:space="preserve"> B5 / Game_Record!$H$2</f>
-        <v>0.88888888888888884</v>
+        <v>0.9</v>
       </c>
       <c r="J5" s="10">
         <f xml:space="preserve"> K5/B5</f>
-        <v>3</v>
+        <v>2.7777777777777777</v>
       </c>
       <c r="K5" s="2">
         <f xml:space="preserve"> (C5 * 5) + (D5 * 3) + (E5 * 1)</f>
-        <v>24</v>
+        <v>25</v>
       </c>
     </row>
     <row r="6" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
@@ -1030,7 +1051,7 @@
       </c>
       <c r="B6" s="2">
         <f xml:space="preserve"> C6 + D6 + E6 + F6</f>
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C6" s="2">
         <f>COUNTIF(Game_Record!C2:C100, "SimpleJack")</f>
@@ -1046,7 +1067,7 @@
       </c>
       <c r="F6" s="2">
         <f>COUNTIF(Game_Record!F2:F100, "SimpleJack")</f>
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="G6" s="3">
         <f xml:space="preserve"> C6 / B6</f>
@@ -1058,11 +1079,11 @@
       </c>
       <c r="I6" s="7">
         <f xml:space="preserve"> B6 / Game_Record!$H$2</f>
-        <v>0.88888888888888884</v>
+        <v>0.9</v>
       </c>
       <c r="J6" s="10">
         <f xml:space="preserve"> K6/B6</f>
-        <v>0.375</v>
+        <v>0.33333333333333331</v>
       </c>
       <c r="K6" s="2">
         <f xml:space="preserve"> (C6 * 5) + (D6 * 3) + (E6 * 1)</f>

</xml_diff>

<commit_message>
Sun Sep 14 23:53:42 EDT 2025
</commit_message>
<xml_diff>
--- a/Doont.xlsx
+++ b/Doont.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29127"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/c92a8a49db0a351e/doont/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cmatt\OneDrive\doont\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="6" documentId="13_ncr:1_{DAA8605B-D9B3-4D9B-BF60-97807A2E23BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B9A290E8-24EE-44DA-B239-011F1CA2090D}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{57F46352-8002-4ED4-B6E9-A83574792ADD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1950" yWindow="1950" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="31965" yWindow="2385" windowWidth="19815" windowHeight="11880" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Game_Record" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="23">
   <si>
     <t>Game #</t>
   </si>
@@ -545,10 +545,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H11"/>
+  <dimension ref="A1:H12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -610,7 +610,7 @@
       </c>
       <c r="H2" s="17">
         <f>COUNTA(Game_Record!B2:B100)</f>
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
@@ -799,6 +799,27 @@
         <v>17</v>
       </c>
       <c r="F11" s="5" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A12" s="5">
+        <f>ROW()-1</f>
+        <v>11</v>
+      </c>
+      <c r="B12" s="6">
+        <v>45914</v>
+      </c>
+      <c r="C12" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="D12" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="E12" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="F12" s="5" t="s">
         <v>18</v>
       </c>
     </row>
@@ -811,8 +832,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E6444F9B-2DCC-4DAB-89DA-045932047514}">
   <dimension ref="A1:K9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -871,11 +892,11 @@
       </c>
       <c r="B2" s="2">
         <f xml:space="preserve"> C2 + D2 + E2 + F2</f>
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C2" s="2">
         <f>COUNTIF(Game_Record!C2:C100, "Doanage")</f>
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D2" s="2">
         <f>COUNTIF(Game_Record!D2:D100, "Doanage")</f>
@@ -891,7 +912,7 @@
       </c>
       <c r="G2" s="3">
         <f xml:space="preserve"> C2 / B2</f>
-        <v>0.75</v>
+        <v>0.77777777777777779</v>
       </c>
       <c r="H2" s="7">
         <f xml:space="preserve"> (C2+D2) / B2</f>
@@ -899,15 +920,15 @@
       </c>
       <c r="I2" s="7">
         <f xml:space="preserve"> B2 / Game_Record!$H$2</f>
-        <v>0.8</v>
+        <v>0.81818181818181823</v>
       </c>
       <c r="J2" s="10">
         <f xml:space="preserve"> K2/B2</f>
-        <v>4.5</v>
+        <v>4.5555555555555554</v>
       </c>
       <c r="K2" s="2">
         <f xml:space="preserve"> (C2 * 5) + (D2 * 3) + (E2 * 1)</f>
-        <v>36</v>
+        <v>41</v>
       </c>
     </row>
     <row r="3" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
@@ -944,7 +965,7 @@
       </c>
       <c r="I3" s="7">
         <f xml:space="preserve"> B3 / Game_Record!$H$2</f>
-        <v>0.6</v>
+        <v>0.54545454545454541</v>
       </c>
       <c r="J3" s="10">
         <f xml:space="preserve"> K3/B3</f>
@@ -961,7 +982,7 @@
       </c>
       <c r="B4" s="2">
         <f xml:space="preserve"> C4 + D4 + E4 + F4</f>
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C4" s="2">
         <f>COUNTIF(Game_Record!C2:C100, "DrSystomatix")</f>
@@ -973,7 +994,7 @@
       </c>
       <c r="E4" s="2">
         <f>COUNTIF(Game_Record!E2:E100, "DrSystomatix")</f>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F4" s="2">
         <f>COUNTIF(Game_Record!F2:F100, "DrSystomatix")</f>
@@ -985,19 +1006,19 @@
       </c>
       <c r="H4" s="7">
         <f xml:space="preserve"> (C4+D4) / B4</f>
-        <v>0.125</v>
+        <v>0.1111111111111111</v>
       </c>
       <c r="I4" s="7">
         <f xml:space="preserve"> B4 / Game_Record!$H$2</f>
-        <v>0.8</v>
+        <v>0.81818181818181823</v>
       </c>
       <c r="J4" s="10">
         <f xml:space="preserve"> K4/B4</f>
-        <v>0.75</v>
+        <v>0.77777777777777779</v>
       </c>
       <c r="K4" s="2">
         <f xml:space="preserve"> (C4 * 5) + (D4 * 3) + (E4 * 1)</f>
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="5" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
@@ -1006,7 +1027,7 @@
       </c>
       <c r="B5" s="2">
         <f xml:space="preserve"> C5 + D5 + E5 + F5</f>
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C5" s="2">
         <f>COUNTIF(Game_Record!C2:C100, "Player1")</f>
@@ -1014,7 +1035,7 @@
       </c>
       <c r="D5" s="2">
         <f>COUNTIF(Game_Record!D2:D100, "Player1")</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E5" s="2">
         <f>COUNTIF(Game_Record!E2:E100, "Player1")</f>
@@ -1026,23 +1047,23 @@
       </c>
       <c r="G5" s="3">
         <f xml:space="preserve"> C5 / B5</f>
-        <v>0.33333333333333331</v>
+        <v>0.3</v>
       </c>
       <c r="H5" s="7">
         <f xml:space="preserve"> (C5+D5) / B5</f>
-        <v>0.55555555555555558</v>
+        <v>0.6</v>
       </c>
       <c r="I5" s="7">
         <f xml:space="preserve"> B5 / Game_Record!$H$2</f>
-        <v>0.9</v>
+        <v>0.90909090909090906</v>
       </c>
       <c r="J5" s="10">
         <f xml:space="preserve"> K5/B5</f>
-        <v>2.7777777777777777</v>
+        <v>2.8</v>
       </c>
       <c r="K5" s="2">
         <f xml:space="preserve"> (C5 * 5) + (D5 * 3) + (E5 * 1)</f>
-        <v>25</v>
+        <v>28</v>
       </c>
     </row>
     <row r="6" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
@@ -1051,7 +1072,7 @@
       </c>
       <c r="B6" s="2">
         <f xml:space="preserve"> C6 + D6 + E6 + F6</f>
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C6" s="2">
         <f>COUNTIF(Game_Record!C2:C100, "SimpleJack")</f>
@@ -1067,7 +1088,7 @@
       </c>
       <c r="F6" s="2">
         <f>COUNTIF(Game_Record!F2:F100, "SimpleJack")</f>
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="G6" s="3">
         <f xml:space="preserve"> C6 / B6</f>
@@ -1079,11 +1100,11 @@
       </c>
       <c r="I6" s="7">
         <f xml:space="preserve"> B6 / Game_Record!$H$2</f>
-        <v>0.9</v>
+        <v>0.90909090909090906</v>
       </c>
       <c r="J6" s="10">
         <f xml:space="preserve"> K6/B6</f>
-        <v>0.33333333333333331</v>
+        <v>0.3</v>
       </c>
       <c r="K6" s="2">
         <f xml:space="preserve"> (C6 * 5) + (D6 * 3) + (E6 * 1)</f>

</xml_diff>

<commit_message>
Wed Sep 24 11:11:53 EDT 2025
</commit_message>
<xml_diff>
--- a/Doont.xlsx
+++ b/Doont.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29231"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cmatt\OneDrive\doont\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{57F46352-8002-4ED4-B6E9-A83574792ADD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E6C7603-37AF-4EA8-BD08-02DDD43CDE24}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="31965" yWindow="2385" windowWidth="19815" windowHeight="11880" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="31965" yWindow="2385" windowWidth="19815" windowHeight="11880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Game_Record" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="23">
   <si>
     <t>Game #</t>
   </si>
@@ -545,10 +545,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H12"/>
+  <dimension ref="A1:H13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G12" sqref="G12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -610,7 +610,7 @@
       </c>
       <c r="H2" s="17">
         <f>COUNTA(Game_Record!B2:B100)</f>
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
@@ -821,6 +821,27 @@
       </c>
       <c r="F12" s="5" t="s">
         <v>18</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A13" s="5">
+        <f>ROW()-1</f>
+        <v>12</v>
+      </c>
+      <c r="B13" s="6">
+        <v>45923</v>
+      </c>
+      <c r="C13" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="D13" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="E13" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="F13" s="5" t="s">
+        <v>19</v>
       </c>
     </row>
   </sheetData>
@@ -832,7 +853,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E6444F9B-2DCC-4DAB-89DA-045932047514}">
   <dimension ref="A1:K9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
@@ -892,11 +913,11 @@
       </c>
       <c r="B2" s="2">
         <f xml:space="preserve"> C2 + D2 + E2 + F2</f>
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C2" s="2">
         <f>COUNTIF(Game_Record!C2:C100, "Doanage")</f>
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D2" s="2">
         <f>COUNTIF(Game_Record!D2:D100, "Doanage")</f>
@@ -912,7 +933,7 @@
       </c>
       <c r="G2" s="3">
         <f xml:space="preserve"> C2 / B2</f>
-        <v>0.77777777777777779</v>
+        <v>0.8</v>
       </c>
       <c r="H2" s="7">
         <f xml:space="preserve"> (C2+D2) / B2</f>
@@ -920,15 +941,15 @@
       </c>
       <c r="I2" s="7">
         <f xml:space="preserve"> B2 / Game_Record!$H$2</f>
-        <v>0.81818181818181823</v>
+        <v>0.83333333333333337</v>
       </c>
       <c r="J2" s="10">
         <f xml:space="preserve"> K2/B2</f>
-        <v>4.5555555555555554</v>
+        <v>4.5999999999999996</v>
       </c>
       <c r="K2" s="2">
         <f xml:space="preserve"> (C2 * 5) + (D2 * 3) + (E2 * 1)</f>
-        <v>41</v>
+        <v>46</v>
       </c>
     </row>
     <row r="3" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
@@ -965,7 +986,7 @@
       </c>
       <c r="I3" s="7">
         <f xml:space="preserve"> B3 / Game_Record!$H$2</f>
-        <v>0.54545454545454541</v>
+        <v>0.5</v>
       </c>
       <c r="J3" s="10">
         <f xml:space="preserve"> K3/B3</f>
@@ -982,7 +1003,7 @@
       </c>
       <c r="B4" s="2">
         <f xml:space="preserve"> C4 + D4 + E4 + F4</f>
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C4" s="2">
         <f>COUNTIF(Game_Record!C2:C100, "DrSystomatix")</f>
@@ -998,7 +1019,7 @@
       </c>
       <c r="F4" s="2">
         <f>COUNTIF(Game_Record!F2:F100, "DrSystomatix")</f>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="G4" s="3">
         <f xml:space="preserve"> C4 / B4</f>
@@ -1006,15 +1027,15 @@
       </c>
       <c r="H4" s="7">
         <f xml:space="preserve"> (C4+D4) / B4</f>
-        <v>0.1111111111111111</v>
+        <v>0.1</v>
       </c>
       <c r="I4" s="7">
         <f xml:space="preserve"> B4 / Game_Record!$H$2</f>
-        <v>0.81818181818181823</v>
+        <v>0.83333333333333337</v>
       </c>
       <c r="J4" s="10">
         <f xml:space="preserve"> K4/B4</f>
-        <v>0.77777777777777779</v>
+        <v>0.7</v>
       </c>
       <c r="K4" s="2">
         <f xml:space="preserve"> (C4 * 5) + (D4 * 3) + (E4 * 1)</f>
@@ -1027,7 +1048,7 @@
       </c>
       <c r="B5" s="2">
         <f xml:space="preserve"> C5 + D5 + E5 + F5</f>
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C5" s="2">
         <f>COUNTIF(Game_Record!C2:C100, "Player1")</f>
@@ -1035,7 +1056,7 @@
       </c>
       <c r="D5" s="2">
         <f>COUNTIF(Game_Record!D2:D100, "Player1")</f>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E5" s="2">
         <f>COUNTIF(Game_Record!E2:E100, "Player1")</f>
@@ -1047,23 +1068,23 @@
       </c>
       <c r="G5" s="3">
         <f xml:space="preserve"> C5 / B5</f>
-        <v>0.3</v>
+        <v>0.27272727272727271</v>
       </c>
       <c r="H5" s="7">
         <f xml:space="preserve"> (C5+D5) / B5</f>
-        <v>0.6</v>
+        <v>0.63636363636363635</v>
       </c>
       <c r="I5" s="7">
         <f xml:space="preserve"> B5 / Game_Record!$H$2</f>
-        <v>0.90909090909090906</v>
+        <v>0.91666666666666663</v>
       </c>
       <c r="J5" s="10">
         <f xml:space="preserve"> K5/B5</f>
-        <v>2.8</v>
+        <v>2.8181818181818183</v>
       </c>
       <c r="K5" s="2">
         <f xml:space="preserve"> (C5 * 5) + (D5 * 3) + (E5 * 1)</f>
-        <v>28</v>
+        <v>31</v>
       </c>
     </row>
     <row r="6" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
@@ -1072,7 +1093,7 @@
       </c>
       <c r="B6" s="2">
         <f xml:space="preserve"> C6 + D6 + E6 + F6</f>
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C6" s="2">
         <f>COUNTIF(Game_Record!C2:C100, "SimpleJack")</f>
@@ -1084,7 +1105,7 @@
       </c>
       <c r="E6" s="2">
         <f>COUNTIF(Game_Record!E2:E100, "SimpleJack")</f>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F6" s="2">
         <f>COUNTIF(Game_Record!F2:F100, "SimpleJack")</f>
@@ -1100,15 +1121,15 @@
       </c>
       <c r="I6" s="7">
         <f xml:space="preserve"> B6 / Game_Record!$H$2</f>
-        <v>0.90909090909090906</v>
+        <v>0.91666666666666663</v>
       </c>
       <c r="J6" s="10">
         <f xml:space="preserve"> K6/B6</f>
-        <v>0.3</v>
+        <v>0.36363636363636365</v>
       </c>
       <c r="K6" s="2">
         <f xml:space="preserve"> (C6 * 5) + (D6 * 3) + (E6 * 1)</f>
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Wed Oct 15 10:31:10 EDT 2025
</commit_message>
<xml_diff>
--- a/Doont.xlsx
+++ b/Doont.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cmatt\OneDrive\doont\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E6C7603-37AF-4EA8-BD08-02DDD43CDE24}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8572C43-4B16-4E1A-8D0E-D4349D5C6C5B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="31965" yWindow="2385" windowWidth="19815" windowHeight="11880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="31965" yWindow="2385" windowWidth="21150" windowHeight="11880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Game_Record" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="23">
   <si>
     <t>Game #</t>
   </si>
@@ -545,10 +545,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H13"/>
+  <dimension ref="A1:H14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+      <selection activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -610,7 +610,7 @@
       </c>
       <c r="H2" s="17">
         <f>COUNTA(Game_Record!B2:B100)</f>
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
@@ -720,7 +720,7 @@
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="5">
-        <f>ROW()-1</f>
+        <f t="shared" ref="A8:A14" si="1">ROW()-1</f>
         <v>7</v>
       </c>
       <c r="B8" s="6">
@@ -741,7 +741,7 @@
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="5">
-        <f>ROW()-1</f>
+        <f t="shared" si="1"/>
         <v>8</v>
       </c>
       <c r="B9" s="6">
@@ -762,7 +762,7 @@
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="5">
-        <f>ROW()-1</f>
+        <f t="shared" si="1"/>
         <v>9</v>
       </c>
       <c r="B10" s="6">
@@ -783,7 +783,7 @@
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="5">
-        <f>ROW()-1</f>
+        <f t="shared" si="1"/>
         <v>10</v>
       </c>
       <c r="B11" s="6">
@@ -804,7 +804,7 @@
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="5">
-        <f>ROW()-1</f>
+        <f t="shared" si="1"/>
         <v>11</v>
       </c>
       <c r="B12" s="6">
@@ -825,7 +825,7 @@
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="5">
-        <f>ROW()-1</f>
+        <f t="shared" si="1"/>
         <v>12</v>
       </c>
       <c r="B13" s="6">
@@ -842,6 +842,27 @@
       </c>
       <c r="F13" s="5" t="s">
         <v>19</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A14" s="5">
+        <f t="shared" si="1"/>
+        <v>13</v>
+      </c>
+      <c r="B14" s="6">
+        <v>45944</v>
+      </c>
+      <c r="C14" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="D14" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="E14" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="F14" s="5" t="s">
+        <v>17</v>
       </c>
     </row>
   </sheetData>
@@ -854,7 +875,7 @@
   <dimension ref="A1:K9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="K4" sqref="K4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -941,7 +962,7 @@
       </c>
       <c r="I2" s="7">
         <f xml:space="preserve"> B2 / Game_Record!$H$2</f>
-        <v>0.83333333333333337</v>
+        <v>0.76923076923076927</v>
       </c>
       <c r="J2" s="10">
         <f xml:space="preserve"> K2/B2</f>
@@ -958,11 +979,11 @@
       </c>
       <c r="B3" s="2">
         <f xml:space="preserve"> C3 + D3 + E3 + F3</f>
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C3" s="2">
         <f>COUNTIF(Game_Record!C2:C100, "SiderFace")</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D3" s="2">
         <f>COUNTIF(Game_Record!D2:D100, "SiderFace")</f>
@@ -978,7 +999,7 @@
       </c>
       <c r="G3" s="3">
         <f xml:space="preserve"> C3 / B3</f>
-        <v>0.16666666666666666</v>
+        <v>0.2857142857142857</v>
       </c>
       <c r="H3" s="7">
         <f xml:space="preserve"> (C3+D3) / B3</f>
@@ -986,15 +1007,15 @@
       </c>
       <c r="I3" s="7">
         <f xml:space="preserve"> B3 / Game_Record!$H$2</f>
-        <v>0.5</v>
+        <v>0.53846153846153844</v>
       </c>
       <c r="J3" s="10">
         <f xml:space="preserve"> K3/B3</f>
-        <v>3.3333333333333335</v>
+        <v>3.5714285714285716</v>
       </c>
       <c r="K3" s="2">
         <f xml:space="preserve"> (C3 * 5) + (D3 * 3) + (E3 * 1)</f>
-        <v>20</v>
+        <v>25</v>
       </c>
     </row>
     <row r="4" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
@@ -1003,7 +1024,7 @@
       </c>
       <c r="B4" s="2">
         <f xml:space="preserve"> C4 + D4 + E4 + F4</f>
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C4" s="2">
         <f>COUNTIF(Game_Record!C2:C100, "DrSystomatix")</f>
@@ -1015,7 +1036,7 @@
       </c>
       <c r="E4" s="2">
         <f>COUNTIF(Game_Record!E2:E100, "DrSystomatix")</f>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="F4" s="2">
         <f>COUNTIF(Game_Record!F2:F100, "DrSystomatix")</f>
@@ -1027,19 +1048,19 @@
       </c>
       <c r="H4" s="7">
         <f xml:space="preserve"> (C4+D4) / B4</f>
-        <v>0.1</v>
+        <v>9.0909090909090912E-2</v>
       </c>
       <c r="I4" s="7">
         <f xml:space="preserve"> B4 / Game_Record!$H$2</f>
-        <v>0.83333333333333337</v>
+        <v>0.84615384615384615</v>
       </c>
       <c r="J4" s="10">
         <f xml:space="preserve"> K4/B4</f>
-        <v>0.7</v>
+        <v>0.72727272727272729</v>
       </c>
       <c r="K4" s="2">
         <f xml:space="preserve"> (C4 * 5) + (D4 * 3) + (E4 * 1)</f>
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="5" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
@@ -1048,7 +1069,7 @@
       </c>
       <c r="B5" s="2">
         <f xml:space="preserve"> C5 + D5 + E5 + F5</f>
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C5" s="2">
         <f>COUNTIF(Game_Record!C2:C100, "Player1")</f>
@@ -1064,23 +1085,23 @@
       </c>
       <c r="F5" s="2">
         <f>COUNTIF(Game_Record!F2:F100, "Player1")</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G5" s="3">
         <f xml:space="preserve"> C5 / B5</f>
-        <v>0.27272727272727271</v>
+        <v>0.25</v>
       </c>
       <c r="H5" s="7">
         <f xml:space="preserve"> (C5+D5) / B5</f>
-        <v>0.63636363636363635</v>
+        <v>0.58333333333333337</v>
       </c>
       <c r="I5" s="7">
         <f xml:space="preserve"> B5 / Game_Record!$H$2</f>
-        <v>0.91666666666666663</v>
+        <v>0.92307692307692313</v>
       </c>
       <c r="J5" s="10">
         <f xml:space="preserve"> K5/B5</f>
-        <v>2.8181818181818183</v>
+        <v>2.5833333333333335</v>
       </c>
       <c r="K5" s="2">
         <f xml:space="preserve"> (C5 * 5) + (D5 * 3) + (E5 * 1)</f>
@@ -1093,7 +1114,7 @@
       </c>
       <c r="B6" s="2">
         <f xml:space="preserve"> C6 + D6 + E6 + F6</f>
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C6" s="2">
         <f>COUNTIF(Game_Record!C2:C100, "SimpleJack")</f>
@@ -1101,7 +1122,7 @@
       </c>
       <c r="D6" s="2">
         <f>COUNTIF(Game_Record!D2:D100, "SimpleJack")</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E6" s="2">
         <f>COUNTIF(Game_Record!E2:E100, "SimpleJack")</f>
@@ -1117,19 +1138,19 @@
       </c>
       <c r="H6" s="7">
         <f xml:space="preserve"> (C6+D6) / B6</f>
-        <v>0</v>
+        <v>8.3333333333333329E-2</v>
       </c>
       <c r="I6" s="7">
         <f xml:space="preserve"> B6 / Game_Record!$H$2</f>
-        <v>0.91666666666666663</v>
+        <v>0.92307692307692313</v>
       </c>
       <c r="J6" s="10">
         <f xml:space="preserve"> K6/B6</f>
-        <v>0.36363636363636365</v>
+        <v>0.58333333333333337</v>
       </c>
       <c r="K6" s="2">
         <f xml:space="preserve"> (C6 * 5) + (D6 * 3) + (E6 * 1)</f>
-        <v>4</v>
+        <v>7</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Tue Oct 21 23:08:48 EDT 2025
</commit_message>
<xml_diff>
--- a/Doont.xlsx
+++ b/Doont.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cmatt\OneDrive\doont\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8572C43-4B16-4E1A-8D0E-D4349D5C6C5B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{632F9ECD-62B0-4CBD-ACE8-9419CAF1FE35}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="31965" yWindow="2385" windowWidth="21150" windowHeight="11880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3165" yWindow="2385" windowWidth="21150" windowHeight="11880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Game_Record" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="23">
   <si>
     <t>Game #</t>
   </si>
@@ -545,10 +545,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H14"/>
+  <dimension ref="A1:H15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A15" sqref="A15"/>
+      <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -610,7 +610,7 @@
       </c>
       <c r="H2" s="17">
         <f>COUNTA(Game_Record!B2:B100)</f>
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
@@ -720,7 +720,7 @@
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="5">
-        <f t="shared" ref="A8:A14" si="1">ROW()-1</f>
+        <f t="shared" ref="A8:A15" si="1">ROW()-1</f>
         <v>7</v>
       </c>
       <c r="B8" s="6">
@@ -863,6 +863,27 @@
       </c>
       <c r="F14" s="5" t="s">
         <v>17</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A15" s="5">
+        <f t="shared" si="1"/>
+        <v>14</v>
+      </c>
+      <c r="B15" s="6">
+        <v>45951</v>
+      </c>
+      <c r="C15" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="D15" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="E15" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="F15" s="5" t="s">
+        <v>18</v>
       </c>
     </row>
   </sheetData>
@@ -934,7 +955,7 @@
       </c>
       <c r="B2" s="2">
         <f xml:space="preserve"> C2 + D2 + E2 + F2</f>
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C2" s="2">
         <f>COUNTIF(Game_Record!C2:C100, "Doanage")</f>
@@ -942,7 +963,7 @@
       </c>
       <c r="D2" s="2">
         <f>COUNTIF(Game_Record!D2:D100, "Doanage")</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E2" s="2">
         <f>COUNTIF(Game_Record!E2:E100, "Doanage")</f>
@@ -954,7 +975,7 @@
       </c>
       <c r="G2" s="3">
         <f xml:space="preserve"> C2 / B2</f>
-        <v>0.8</v>
+        <v>0.72727272727272729</v>
       </c>
       <c r="H2" s="7">
         <f xml:space="preserve"> (C2+D2) / B2</f>
@@ -962,15 +983,15 @@
       </c>
       <c r="I2" s="7">
         <f xml:space="preserve"> B2 / Game_Record!$H$2</f>
-        <v>0.76923076923076927</v>
+        <v>0.7857142857142857</v>
       </c>
       <c r="J2" s="10">
         <f xml:space="preserve"> K2/B2</f>
-        <v>4.5999999999999996</v>
+        <v>4.4545454545454541</v>
       </c>
       <c r="K2" s="2">
         <f xml:space="preserve"> (C2 * 5) + (D2 * 3) + (E2 * 1)</f>
-        <v>46</v>
+        <v>49</v>
       </c>
     </row>
     <row r="3" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
@@ -979,11 +1000,11 @@
       </c>
       <c r="B3" s="2">
         <f xml:space="preserve"> C3 + D3 + E3 + F3</f>
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C3" s="2">
         <f>COUNTIF(Game_Record!C2:C100, "SiderFace")</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D3" s="2">
         <f>COUNTIF(Game_Record!D2:D100, "SiderFace")</f>
@@ -999,7 +1020,7 @@
       </c>
       <c r="G3" s="3">
         <f xml:space="preserve"> C3 / B3</f>
-        <v>0.2857142857142857</v>
+        <v>0.375</v>
       </c>
       <c r="H3" s="7">
         <f xml:space="preserve"> (C3+D3) / B3</f>
@@ -1007,15 +1028,15 @@
       </c>
       <c r="I3" s="7">
         <f xml:space="preserve"> B3 / Game_Record!$H$2</f>
-        <v>0.53846153846153844</v>
+        <v>0.5714285714285714</v>
       </c>
       <c r="J3" s="10">
         <f xml:space="preserve"> K3/B3</f>
-        <v>3.5714285714285716</v>
+        <v>3.75</v>
       </c>
       <c r="K3" s="2">
         <f xml:space="preserve"> (C3 * 5) + (D3 * 3) + (E3 * 1)</f>
-        <v>25</v>
+        <v>30</v>
       </c>
     </row>
     <row r="4" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
@@ -1024,7 +1045,7 @@
       </c>
       <c r="B4" s="2">
         <f xml:space="preserve"> C4 + D4 + E4 + F4</f>
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C4" s="2">
         <f>COUNTIF(Game_Record!C2:C100, "DrSystomatix")</f>
@@ -1036,7 +1057,7 @@
       </c>
       <c r="E4" s="2">
         <f>COUNTIF(Game_Record!E2:E100, "DrSystomatix")</f>
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="F4" s="2">
         <f>COUNTIF(Game_Record!F2:F100, "DrSystomatix")</f>
@@ -1048,19 +1069,19 @@
       </c>
       <c r="H4" s="7">
         <f xml:space="preserve"> (C4+D4) / B4</f>
-        <v>9.0909090909090912E-2</v>
+        <v>8.3333333333333329E-2</v>
       </c>
       <c r="I4" s="7">
         <f xml:space="preserve"> B4 / Game_Record!$H$2</f>
-        <v>0.84615384615384615</v>
+        <v>0.8571428571428571</v>
       </c>
       <c r="J4" s="10">
         <f xml:space="preserve"> K4/B4</f>
-        <v>0.72727272727272729</v>
+        <v>0.75</v>
       </c>
       <c r="K4" s="2">
         <f xml:space="preserve"> (C4 * 5) + (D4 * 3) + (E4 * 1)</f>
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="5" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
@@ -1097,7 +1118,7 @@
       </c>
       <c r="I5" s="7">
         <f xml:space="preserve"> B5 / Game_Record!$H$2</f>
-        <v>0.92307692307692313</v>
+        <v>0.8571428571428571</v>
       </c>
       <c r="J5" s="10">
         <f xml:space="preserve"> K5/B5</f>
@@ -1114,7 +1135,7 @@
       </c>
       <c r="B6" s="2">
         <f xml:space="preserve"> C6 + D6 + E6 + F6</f>
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C6" s="2">
         <f>COUNTIF(Game_Record!C2:C100, "SimpleJack")</f>
@@ -1130,7 +1151,7 @@
       </c>
       <c r="F6" s="2">
         <f>COUNTIF(Game_Record!F2:F100, "SimpleJack")</f>
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="G6" s="3">
         <f xml:space="preserve"> C6 / B6</f>
@@ -1138,15 +1159,15 @@
       </c>
       <c r="H6" s="7">
         <f xml:space="preserve"> (C6+D6) / B6</f>
-        <v>8.3333333333333329E-2</v>
+        <v>7.6923076923076927E-2</v>
       </c>
       <c r="I6" s="7">
         <f xml:space="preserve"> B6 / Game_Record!$H$2</f>
-        <v>0.92307692307692313</v>
+        <v>0.9285714285714286</v>
       </c>
       <c r="J6" s="10">
         <f xml:space="preserve"> K6/B6</f>
-        <v>0.58333333333333337</v>
+        <v>0.53846153846153844</v>
       </c>
       <c r="K6" s="2">
         <f xml:space="preserve"> (C6 * 5) + (D6 * 3) + (E6 * 1)</f>

</xml_diff>

<commit_message>
Fri Nov 21 00:13:30 EST 2025
</commit_message>
<xml_diff>
--- a/Doont.xlsx
+++ b/Doont.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29328"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cmatt\OneDrive\doont\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{632F9ECD-62B0-4CBD-ACE8-9419CAF1FE35}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18B6BD4D-5295-43D3-815F-9AFCAB53AD05}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3165" yWindow="2385" windowWidth="21150" windowHeight="11880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="32880" yWindow="1350" windowWidth="21150" windowHeight="11880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Game_Record" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="23">
   <si>
     <t>Game #</t>
   </si>
@@ -545,10 +545,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H15"/>
+  <dimension ref="A1:H17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G15" sqref="G15"/>
+      <selection activeCell="G17" sqref="G17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -610,7 +610,7 @@
       </c>
       <c r="H2" s="17">
         <f>COUNTA(Game_Record!B2:B100)</f>
-        <v>14</v>
+        <v>16</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
@@ -720,7 +720,7 @@
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="5">
-        <f t="shared" ref="A8:A15" si="1">ROW()-1</f>
+        <f t="shared" ref="A8:A17" si="1">ROW()-1</f>
         <v>7</v>
       </c>
       <c r="B8" s="6">
@@ -883,6 +883,48 @@
         <v>19</v>
       </c>
       <c r="F15" s="5" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A16" s="5">
+        <f t="shared" si="1"/>
+        <v>15</v>
+      </c>
+      <c r="B16" s="6">
+        <v>45956</v>
+      </c>
+      <c r="C16" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="D16" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="E16" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="F16" s="5" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A17" s="5">
+        <f t="shared" si="1"/>
+        <v>16</v>
+      </c>
+      <c r="B17" s="6">
+        <v>45982</v>
+      </c>
+      <c r="C17" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="D17" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="E17" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="F17" s="5" t="s">
         <v>18</v>
       </c>
     </row>
@@ -955,7 +997,7 @@
       </c>
       <c r="B2" s="2">
         <f xml:space="preserve"> C2 + D2 + E2 + F2</f>
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C2" s="2">
         <f>COUNTIF(Game_Record!C2:C100, "Doanage")</f>
@@ -967,7 +1009,7 @@
       </c>
       <c r="E2" s="2">
         <f>COUNTIF(Game_Record!E2:E100, "Doanage")</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F2" s="2">
         <f>COUNTIF(Game_Record!F2:F100, "Doanage")</f>
@@ -975,23 +1017,23 @@
       </c>
       <c r="G2" s="3">
         <f xml:space="preserve"> C2 / B2</f>
-        <v>0.72727272727272729</v>
+        <v>0.66666666666666663</v>
       </c>
       <c r="H2" s="7">
         <f xml:space="preserve"> (C2+D2) / B2</f>
-        <v>1</v>
+        <v>0.91666666666666663</v>
       </c>
       <c r="I2" s="7">
         <f xml:space="preserve"> B2 / Game_Record!$H$2</f>
-        <v>0.7857142857142857</v>
+        <v>0.75</v>
       </c>
       <c r="J2" s="10">
         <f xml:space="preserve"> K2/B2</f>
-        <v>4.4545454545454541</v>
+        <v>4.166666666666667</v>
       </c>
       <c r="K2" s="2">
         <f xml:space="preserve"> (C2 * 5) + (D2 * 3) + (E2 * 1)</f>
-        <v>49</v>
+        <v>50</v>
       </c>
     </row>
     <row r="3" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
@@ -1000,11 +1042,11 @@
       </c>
       <c r="B3" s="2">
         <f xml:space="preserve"> C3 + D3 + E3 + F3</f>
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="C3" s="2">
         <f>COUNTIF(Game_Record!C2:C100, "SiderFace")</f>
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="D3" s="2">
         <f>COUNTIF(Game_Record!D2:D100, "SiderFace")</f>
@@ -1020,7 +1062,7 @@
       </c>
       <c r="G3" s="3">
         <f xml:space="preserve"> C3 / B3</f>
-        <v>0.375</v>
+        <v>0.5</v>
       </c>
       <c r="H3" s="7">
         <f xml:space="preserve"> (C3+D3) / B3</f>
@@ -1028,15 +1070,15 @@
       </c>
       <c r="I3" s="7">
         <f xml:space="preserve"> B3 / Game_Record!$H$2</f>
-        <v>0.5714285714285714</v>
+        <v>0.625</v>
       </c>
       <c r="J3" s="10">
         <f xml:space="preserve"> K3/B3</f>
-        <v>3.75</v>
+        <v>4</v>
       </c>
       <c r="K3" s="2">
         <f xml:space="preserve"> (C3 * 5) + (D3 * 3) + (E3 * 1)</f>
-        <v>30</v>
+        <v>40</v>
       </c>
     </row>
     <row r="4" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
@@ -1045,7 +1087,7 @@
       </c>
       <c r="B4" s="2">
         <f xml:space="preserve"> C4 + D4 + E4 + F4</f>
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C4" s="2">
         <f>COUNTIF(Game_Record!C2:C100, "DrSystomatix")</f>
@@ -1053,7 +1095,7 @@
       </c>
       <c r="D4" s="2">
         <f>COUNTIF(Game_Record!D2:D100, "DrSystomatix")</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E4" s="2">
         <f>COUNTIF(Game_Record!E2:E100, "DrSystomatix")</f>
@@ -1069,19 +1111,19 @@
       </c>
       <c r="H4" s="7">
         <f xml:space="preserve"> (C4+D4) / B4</f>
-        <v>8.3333333333333329E-2</v>
+        <v>0.15384615384615385</v>
       </c>
       <c r="I4" s="7">
         <f xml:space="preserve"> B4 / Game_Record!$H$2</f>
-        <v>0.8571428571428571</v>
+        <v>0.8125</v>
       </c>
       <c r="J4" s="10">
         <f xml:space="preserve"> K4/B4</f>
-        <v>0.75</v>
+        <v>0.92307692307692313</v>
       </c>
       <c r="K4" s="2">
         <f xml:space="preserve"> (C4 * 5) + (D4 * 3) + (E4 * 1)</f>
-        <v>9</v>
+        <v>12</v>
       </c>
     </row>
     <row r="5" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
@@ -1090,7 +1132,7 @@
       </c>
       <c r="B5" s="2">
         <f xml:space="preserve"> C5 + D5 + E5 + F5</f>
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="C5" s="2">
         <f>COUNTIF(Game_Record!C2:C100, "Player1")</f>
@@ -1098,7 +1140,7 @@
       </c>
       <c r="D5" s="2">
         <f>COUNTIF(Game_Record!D2:D100, "Player1")</f>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="E5" s="2">
         <f>COUNTIF(Game_Record!E2:E100, "Player1")</f>
@@ -1106,27 +1148,27 @@
       </c>
       <c r="F5" s="2">
         <f>COUNTIF(Game_Record!F2:F100, "Player1")</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G5" s="3">
         <f xml:space="preserve"> C5 / B5</f>
-        <v>0.25</v>
+        <v>0.21428571428571427</v>
       </c>
       <c r="H5" s="7">
         <f xml:space="preserve"> (C5+D5) / B5</f>
-        <v>0.58333333333333337</v>
+        <v>0.5714285714285714</v>
       </c>
       <c r="I5" s="7">
         <f xml:space="preserve"> B5 / Game_Record!$H$2</f>
-        <v>0.8571428571428571</v>
+        <v>0.875</v>
       </c>
       <c r="J5" s="10">
         <f xml:space="preserve"> K5/B5</f>
-        <v>2.5833333333333335</v>
+        <v>2.4285714285714284</v>
       </c>
       <c r="K5" s="2">
         <f xml:space="preserve"> (C5 * 5) + (D5 * 3) + (E5 * 1)</f>
-        <v>31</v>
+        <v>34</v>
       </c>
     </row>
     <row r="6" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
@@ -1135,7 +1177,7 @@
       </c>
       <c r="B6" s="2">
         <f xml:space="preserve"> C6 + D6 + E6 + F6</f>
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="C6" s="2">
         <f>COUNTIF(Game_Record!C2:C100, "SimpleJack")</f>
@@ -1147,11 +1189,11 @@
       </c>
       <c r="E6" s="2">
         <f>COUNTIF(Game_Record!E2:E100, "SimpleJack")</f>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="F6" s="2">
         <f>COUNTIF(Game_Record!F2:F100, "SimpleJack")</f>
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="G6" s="3">
         <f xml:space="preserve"> C6 / B6</f>
@@ -1159,19 +1201,19 @@
       </c>
       <c r="H6" s="7">
         <f xml:space="preserve"> (C6+D6) / B6</f>
-        <v>7.6923076923076927E-2</v>
+        <v>6.6666666666666666E-2</v>
       </c>
       <c r="I6" s="7">
         <f xml:space="preserve"> B6 / Game_Record!$H$2</f>
-        <v>0.9285714285714286</v>
+        <v>0.9375</v>
       </c>
       <c r="J6" s="10">
         <f xml:space="preserve"> K6/B6</f>
-        <v>0.53846153846153844</v>
+        <v>0.53333333333333333</v>
       </c>
       <c r="K6" s="2">
         <f xml:space="preserve"> (C6 * 5) + (D6 * 3) + (E6 * 1)</f>
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Sat Jan 31 17:09:21 EST 2026
</commit_message>
<xml_diff>
--- a/Doont.xlsx
+++ b/Doont.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29628"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cmatt\OneDrive\doont\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18B6BD4D-5295-43D3-815F-9AFCAB53AD05}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05028BDD-ABC3-4908-8F2D-D06A1688B815}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="32880" yWindow="1350" windowWidth="21150" windowHeight="11880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2835" yWindow="0" windowWidth="23550" windowHeight="11880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Game_Record" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="25">
   <si>
     <t>Game #</t>
   </si>
@@ -106,6 +106,12 @@
   </si>
   <si>
     <t>Total Games Played</t>
+  </si>
+  <si>
+    <t>Start</t>
+  </si>
+  <si>
+    <t>End</t>
   </si>
 </sst>
 </file>
@@ -212,7 +218,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -263,6 +269,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -545,10 +554,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H17"/>
+  <dimension ref="A1:J21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G17" sqref="G17"/>
+      <selection activeCell="M11" sqref="M11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -561,10 +570,12 @@
     <col min="6" max="6" width="17.42578125" style="5" customWidth="1"/>
     <col min="7" max="7" width="9.140625" style="5"/>
     <col min="8" max="8" width="25.5703125" style="5" customWidth="1"/>
-    <col min="9" max="16384" width="9.140625" style="5"/>
+    <col min="9" max="9" width="13.5703125" style="5" customWidth="1"/>
+    <col min="10" max="10" width="12.85546875" style="5" customWidth="1"/>
+    <col min="11" max="16384" width="9.140625" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A1" s="14" t="s">
         <v>0</v>
       </c>
@@ -587,8 +598,14 @@
       <c r="H1" s="14" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="2" spans="1:8" ht="21" x14ac:dyDescent="0.25">
+      <c r="I1" s="14" t="s">
+        <v>23</v>
+      </c>
+      <c r="J1" s="14" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" ht="21" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
         <f>ROW()-1</f>
         <v>1</v>
@@ -609,11 +626,11 @@
         <v>18</v>
       </c>
       <c r="H2" s="17">
-        <f>COUNTA(Game_Record!B2:B100)</f>
-        <v>16</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+        <f>COUNTA(Game_Record!B2:B101)</f>
+        <v>20</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
         <f t="shared" ref="A3:A7" si="0">ROW()-1</f>
         <v>2</v>
@@ -634,7 +651,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
         <f t="shared" si="0"/>
         <v>3</v>
@@ -655,7 +672,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
         <f t="shared" si="0"/>
         <v>4</v>
@@ -676,7 +693,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
         <f t="shared" si="0"/>
         <v>5</v>
@@ -697,7 +714,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
         <f t="shared" si="0"/>
         <v>6</v>
@@ -718,9 +735,9 @@
         <v>18</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="5">
-        <f t="shared" ref="A8:A17" si="1">ROW()-1</f>
+        <f t="shared" ref="A8:A21" si="1">ROW()-1</f>
         <v>7</v>
       </c>
       <c r="B8" s="6">
@@ -739,7 +756,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" s="5">
         <f t="shared" si="1"/>
         <v>8</v>
@@ -760,7 +777,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" s="5">
         <f t="shared" si="1"/>
         <v>9</v>
@@ -781,7 +798,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" s="5">
         <f t="shared" si="1"/>
         <v>10</v>
@@ -802,7 +819,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" s="5">
         <f t="shared" si="1"/>
         <v>11</v>
@@ -823,7 +840,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" s="5">
         <f t="shared" si="1"/>
         <v>12</v>
@@ -844,7 +861,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" s="5">
         <f t="shared" si="1"/>
         <v>13</v>
@@ -865,7 +882,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" s="5">
         <f t="shared" si="1"/>
         <v>14</v>
@@ -886,7 +903,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" s="5">
         <f t="shared" si="1"/>
         <v>15</v>
@@ -907,13 +924,13 @@
         <v>17</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" s="5">
         <f t="shared" si="1"/>
         <v>16</v>
       </c>
       <c r="B17" s="6">
-        <v>45982</v>
+        <v>45981</v>
       </c>
       <c r="C17" s="5" t="s">
         <v>16</v>
@@ -926,6 +943,96 @@
       </c>
       <c r="F17" s="5" t="s">
         <v>18</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A18" s="5">
+        <f t="shared" si="1"/>
+        <v>17</v>
+      </c>
+      <c r="B18" s="6">
+        <v>46006</v>
+      </c>
+      <c r="C18" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="D18" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="E18" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="F18" s="5" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A19" s="5">
+        <f t="shared" si="1"/>
+        <v>18</v>
+      </c>
+      <c r="B19" s="6">
+        <v>46027</v>
+      </c>
+      <c r="C19" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="D19" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="E19" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="F19" s="5" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A20" s="5">
+        <f t="shared" si="1"/>
+        <v>19</v>
+      </c>
+      <c r="B20" s="6">
+        <v>46032</v>
+      </c>
+      <c r="C20" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="D20" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="E20" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="F20" s="5" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A21" s="5">
+        <f t="shared" si="1"/>
+        <v>20</v>
+      </c>
+      <c r="B21" s="6">
+        <v>46050</v>
+      </c>
+      <c r="C21" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="D21" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="E21" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="F21" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="I21" s="18">
+        <v>0.87222222222222223</v>
+      </c>
+      <c r="J21" s="18">
+        <v>0.9458333333333333</v>
       </c>
     </row>
   </sheetData>
@@ -938,7 +1045,7 @@
   <dimension ref="A1:K9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K4" sqref="K4"/>
+      <selection activeCell="K7" sqref="K7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -997,43 +1104,43 @@
       </c>
       <c r="B2" s="2">
         <f xml:space="preserve"> C2 + D2 + E2 + F2</f>
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="C2" s="2">
-        <f>COUNTIF(Game_Record!C2:C100, "Doanage")</f>
+        <f>COUNTIF(Game_Record!C2:C101, "Doanage")</f>
         <v>8</v>
       </c>
       <c r="D2" s="2">
-        <f>COUNTIF(Game_Record!D2:D100, "Doanage")</f>
+        <f>COUNTIF(Game_Record!D2:D101, "Doanage")</f>
         <v>3</v>
       </c>
       <c r="E2" s="2">
-        <f>COUNTIF(Game_Record!E2:E100, "Doanage")</f>
+        <f>COUNTIF(Game_Record!E2:E101, "Doanage")</f>
+        <v>2</v>
+      </c>
+      <c r="F2" s="2">
+        <f>COUNTIF(Game_Record!F2:F101, "Doanage")</f>
         <v>1</v>
-      </c>
-      <c r="F2" s="2">
-        <f>COUNTIF(Game_Record!F2:F100, "Doanage")</f>
-        <v>0</v>
       </c>
       <c r="G2" s="3">
         <f xml:space="preserve"> C2 / B2</f>
-        <v>0.66666666666666663</v>
+        <v>0.5714285714285714</v>
       </c>
       <c r="H2" s="7">
         <f xml:space="preserve"> (C2+D2) / B2</f>
-        <v>0.91666666666666663</v>
+        <v>0.7857142857142857</v>
       </c>
       <c r="I2" s="7">
         <f xml:space="preserve"> B2 / Game_Record!$H$2</f>
-        <v>0.75</v>
+        <v>0.7</v>
       </c>
       <c r="J2" s="10">
         <f xml:space="preserve"> K2/B2</f>
-        <v>4.166666666666667</v>
+        <v>3.6428571428571428</v>
       </c>
       <c r="K2" s="2">
         <f xml:space="preserve"> (C2 * 5) + (D2 * 3) + (E2 * 1)</f>
-        <v>50</v>
+        <v>51</v>
       </c>
     </row>
     <row r="3" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
@@ -1042,27 +1149,27 @@
       </c>
       <c r="B3" s="2">
         <f xml:space="preserve"> C3 + D3 + E3 + F3</f>
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="C3" s="2">
-        <f>COUNTIF(Game_Record!C2:C100, "SiderFace")</f>
+        <f>COUNTIF(Game_Record!C2:C101, "SiderFace")</f>
+        <v>8</v>
+      </c>
+      <c r="D3" s="2">
+        <f>COUNTIF(Game_Record!D2:D101, "SiderFace")</f>
         <v>5</v>
       </c>
-      <c r="D3" s="2">
-        <f>COUNTIF(Game_Record!D2:D100, "SiderFace")</f>
-        <v>5</v>
-      </c>
       <c r="E3" s="2">
-        <f>COUNTIF(Game_Record!E2:E100, "SiderFace")</f>
+        <f>COUNTIF(Game_Record!E2:E101, "SiderFace")</f>
         <v>0</v>
       </c>
       <c r="F3" s="2">
-        <f>COUNTIF(Game_Record!F2:F100, "SiderFace")</f>
+        <f>COUNTIF(Game_Record!F2:F101, "SiderFace")</f>
         <v>0</v>
       </c>
       <c r="G3" s="3">
         <f xml:space="preserve"> C3 / B3</f>
-        <v>0.5</v>
+        <v>0.61538461538461542</v>
       </c>
       <c r="H3" s="7">
         <f xml:space="preserve"> (C3+D3) / B3</f>
@@ -1070,15 +1177,15 @@
       </c>
       <c r="I3" s="7">
         <f xml:space="preserve"> B3 / Game_Record!$H$2</f>
-        <v>0.625</v>
+        <v>0.65</v>
       </c>
       <c r="J3" s="10">
         <f xml:space="preserve"> K3/B3</f>
-        <v>4</v>
+        <v>4.2307692307692308</v>
       </c>
       <c r="K3" s="2">
         <f xml:space="preserve"> (C3 * 5) + (D3 * 3) + (E3 * 1)</f>
-        <v>40</v>
+        <v>55</v>
       </c>
     </row>
     <row r="4" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
@@ -1087,23 +1194,23 @@
       </c>
       <c r="B4" s="2">
         <f xml:space="preserve"> C4 + D4 + E4 + F4</f>
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="C4" s="2">
-        <f>COUNTIF(Game_Record!C2:C100, "DrSystomatix")</f>
+        <f>COUNTIF(Game_Record!C2:C101, "DrSystomatix")</f>
         <v>0</v>
       </c>
       <c r="D4" s="2">
-        <f>COUNTIF(Game_Record!D2:D100, "DrSystomatix")</f>
-        <v>2</v>
+        <f>COUNTIF(Game_Record!D2:D101, "DrSystomatix")</f>
+        <v>3</v>
       </c>
       <c r="E4" s="2">
-        <f>COUNTIF(Game_Record!E2:E100, "DrSystomatix")</f>
+        <f>COUNTIF(Game_Record!E2:E101, "DrSystomatix")</f>
+        <v>7</v>
+      </c>
+      <c r="F4" s="2">
+        <f>COUNTIF(Game_Record!F2:F101, "DrSystomatix")</f>
         <v>6</v>
-      </c>
-      <c r="F4" s="2">
-        <f>COUNTIF(Game_Record!F2:F100, "DrSystomatix")</f>
-        <v>5</v>
       </c>
       <c r="G4" s="3">
         <f xml:space="preserve"> C4 / B4</f>
@@ -1111,19 +1218,19 @@
       </c>
       <c r="H4" s="7">
         <f xml:space="preserve"> (C4+D4) / B4</f>
-        <v>0.15384615384615385</v>
+        <v>0.1875</v>
       </c>
       <c r="I4" s="7">
         <f xml:space="preserve"> B4 / Game_Record!$H$2</f>
-        <v>0.8125</v>
+        <v>0.8</v>
       </c>
       <c r="J4" s="10">
         <f xml:space="preserve"> K4/B4</f>
-        <v>0.92307692307692313</v>
+        <v>1</v>
       </c>
       <c r="K4" s="2">
         <f xml:space="preserve"> (C4 * 5) + (D4 * 3) + (E4 * 1)</f>
-        <v>12</v>
+        <v>16</v>
       </c>
     </row>
     <row r="5" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
@@ -1132,43 +1239,43 @@
       </c>
       <c r="B5" s="2">
         <f xml:space="preserve"> C5 + D5 + E5 + F5</f>
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="C5" s="2">
-        <f>COUNTIF(Game_Record!C2:C100, "Player1")</f>
-        <v>3</v>
+        <f>COUNTIF(Game_Record!C2:C101, "Player1")</f>
+        <v>4</v>
       </c>
       <c r="D5" s="2">
-        <f>COUNTIF(Game_Record!D2:D100, "Player1")</f>
+        <f>COUNTIF(Game_Record!D2:D101, "Player1")</f>
+        <v>7</v>
+      </c>
+      <c r="E5" s="2">
+        <f>COUNTIF(Game_Record!E2:E101, "Player1")</f>
         <v>5</v>
       </c>
-      <c r="E5" s="2">
-        <f>COUNTIF(Game_Record!E2:E100, "Player1")</f>
-        <v>4</v>
-      </c>
       <c r="F5" s="2">
-        <f>COUNTIF(Game_Record!F2:F100, "Player1")</f>
+        <f>COUNTIF(Game_Record!F2:F101, "Player1")</f>
         <v>2</v>
       </c>
       <c r="G5" s="3">
         <f xml:space="preserve"> C5 / B5</f>
-        <v>0.21428571428571427</v>
+        <v>0.22222222222222221</v>
       </c>
       <c r="H5" s="7">
         <f xml:space="preserve"> (C5+D5) / B5</f>
-        <v>0.5714285714285714</v>
+        <v>0.61111111111111116</v>
       </c>
       <c r="I5" s="7">
         <f xml:space="preserve"> B5 / Game_Record!$H$2</f>
-        <v>0.875</v>
+        <v>0.9</v>
       </c>
       <c r="J5" s="10">
         <f xml:space="preserve"> K5/B5</f>
-        <v>2.4285714285714284</v>
+        <v>2.5555555555555554</v>
       </c>
       <c r="K5" s="2">
         <f xml:space="preserve"> (C5 * 5) + (D5 * 3) + (E5 * 1)</f>
-        <v>34</v>
+        <v>46</v>
       </c>
     </row>
     <row r="6" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
@@ -1177,23 +1284,23 @@
       </c>
       <c r="B6" s="2">
         <f xml:space="preserve"> C6 + D6 + E6 + F6</f>
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="C6" s="2">
-        <f>COUNTIF(Game_Record!C2:C100, "SimpleJack")</f>
+        <f>COUNTIF(Game_Record!C2:C101, "SimpleJack")</f>
         <v>0</v>
       </c>
       <c r="D6" s="2">
-        <f>COUNTIF(Game_Record!D2:D100, "SimpleJack")</f>
-        <v>1</v>
+        <f>COUNTIF(Game_Record!D2:D101, "SimpleJack")</f>
+        <v>2</v>
       </c>
       <c r="E6" s="2">
-        <f>COUNTIF(Game_Record!E2:E100, "SimpleJack")</f>
-        <v>5</v>
+        <f>COUNTIF(Game_Record!E2:E101, "SimpleJack")</f>
+        <v>6</v>
       </c>
       <c r="F6" s="2">
-        <f>COUNTIF(Game_Record!F2:F100, "SimpleJack")</f>
-        <v>9</v>
+        <f>COUNTIF(Game_Record!F2:F101, "SimpleJack")</f>
+        <v>11</v>
       </c>
       <c r="G6" s="3">
         <f xml:space="preserve"> C6 / B6</f>
@@ -1201,19 +1308,19 @@
       </c>
       <c r="H6" s="7">
         <f xml:space="preserve"> (C6+D6) / B6</f>
-        <v>6.6666666666666666E-2</v>
+        <v>0.10526315789473684</v>
       </c>
       <c r="I6" s="7">
         <f xml:space="preserve"> B6 / Game_Record!$H$2</f>
-        <v>0.9375</v>
+        <v>0.95</v>
       </c>
       <c r="J6" s="10">
         <f xml:space="preserve"> K6/B6</f>
-        <v>0.53333333333333333</v>
+        <v>0.63157894736842102</v>
       </c>
       <c r="K6" s="2">
         <f xml:space="preserve"> (C6 * 5) + (D6 * 3) + (E6 * 1)</f>
-        <v>8</v>
+        <v>12</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Thu Feb  5 23:00:37 EST 2026
</commit_message>
<xml_diff>
--- a/Doont.xlsx
+++ b/Doont.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cmatt\OneDrive\doont\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05028BDD-ABC3-4908-8F2D-D06A1688B815}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44F2C5FC-C40F-4254-B948-D47E3F0FB446}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2835" yWindow="0" windowWidth="23550" windowHeight="11880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4365" yWindow="1110" windowWidth="23550" windowHeight="11880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Game_Record" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="25">
   <si>
     <t>Game #</t>
   </si>
@@ -554,10 +554,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J21"/>
+  <dimension ref="A1:J22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M11" sqref="M11"/>
+      <selection activeCell="A23" sqref="A23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -627,7 +627,7 @@
       </c>
       <c r="H2" s="17">
         <f>COUNTA(Game_Record!B2:B101)</f>
-        <v>20</v>
+        <v>21</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
@@ -737,7 +737,7 @@
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="5">
-        <f t="shared" ref="A8:A21" si="1">ROW()-1</f>
+        <f t="shared" ref="A8:A22" si="1">ROW()-1</f>
         <v>7</v>
       </c>
       <c r="B8" s="6">
@@ -1033,6 +1033,33 @@
       </c>
       <c r="J21" s="18">
         <v>0.9458333333333333</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A22" s="5">
+        <f t="shared" si="1"/>
+        <v>21</v>
+      </c>
+      <c r="B22" s="6">
+        <v>46058</v>
+      </c>
+      <c r="C22" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="D22" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="E22" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="F22" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="I22" s="18">
+        <v>0.87777777777777777</v>
+      </c>
+      <c r="J22" s="18">
+        <v>0.95763888888888893</v>
       </c>
     </row>
   </sheetData>
@@ -1104,7 +1131,7 @@
       </c>
       <c r="B2" s="2">
         <f xml:space="preserve"> C2 + D2 + E2 + F2</f>
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C2" s="2">
         <f>COUNTIF(Game_Record!C2:C101, "Doanage")</f>
@@ -1116,7 +1143,7 @@
       </c>
       <c r="E2" s="2">
         <f>COUNTIF(Game_Record!E2:E101, "Doanage")</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F2" s="2">
         <f>COUNTIF(Game_Record!F2:F101, "Doanage")</f>
@@ -1124,23 +1151,23 @@
       </c>
       <c r="G2" s="3">
         <f xml:space="preserve"> C2 / B2</f>
-        <v>0.5714285714285714</v>
+        <v>0.53333333333333333</v>
       </c>
       <c r="H2" s="7">
         <f xml:space="preserve"> (C2+D2) / B2</f>
-        <v>0.7857142857142857</v>
+        <v>0.73333333333333328</v>
       </c>
       <c r="I2" s="7">
         <f xml:space="preserve"> B2 / Game_Record!$H$2</f>
-        <v>0.7</v>
+        <v>0.7142857142857143</v>
       </c>
       <c r="J2" s="10">
         <f xml:space="preserve"> K2/B2</f>
-        <v>3.6428571428571428</v>
+        <v>3.4666666666666668</v>
       </c>
       <c r="K2" s="2">
         <f xml:space="preserve"> (C2 * 5) + (D2 * 3) + (E2 * 1)</f>
-        <v>51</v>
+        <v>52</v>
       </c>
     </row>
     <row r="3" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
@@ -1149,7 +1176,7 @@
       </c>
       <c r="B3" s="2">
         <f xml:space="preserve"> C3 + D3 + E3 + F3</f>
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C3" s="2">
         <f>COUNTIF(Game_Record!C2:C101, "SiderFace")</f>
@@ -1165,23 +1192,23 @@
       </c>
       <c r="F3" s="2">
         <f>COUNTIF(Game_Record!F2:F101, "SiderFace")</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G3" s="3">
         <f xml:space="preserve"> C3 / B3</f>
-        <v>0.61538461538461542</v>
+        <v>0.5714285714285714</v>
       </c>
       <c r="H3" s="7">
         <f xml:space="preserve"> (C3+D3) / B3</f>
-        <v>1</v>
+        <v>0.9285714285714286</v>
       </c>
       <c r="I3" s="7">
         <f xml:space="preserve"> B3 / Game_Record!$H$2</f>
-        <v>0.65</v>
+        <v>0.66666666666666663</v>
       </c>
       <c r="J3" s="10">
         <f xml:space="preserve"> K3/B3</f>
-        <v>4.2307692307692308</v>
+        <v>3.9285714285714284</v>
       </c>
       <c r="K3" s="2">
         <f xml:space="preserve"> (C3 * 5) + (D3 * 3) + (E3 * 1)</f>
@@ -1194,7 +1221,7 @@
       </c>
       <c r="B4" s="2">
         <f xml:space="preserve"> C4 + D4 + E4 + F4</f>
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C4" s="2">
         <f>COUNTIF(Game_Record!C2:C101, "DrSystomatix")</f>
@@ -1202,7 +1229,7 @@
       </c>
       <c r="D4" s="2">
         <f>COUNTIF(Game_Record!D2:D101, "DrSystomatix")</f>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E4" s="2">
         <f>COUNTIF(Game_Record!E2:E101, "DrSystomatix")</f>
@@ -1218,19 +1245,19 @@
       </c>
       <c r="H4" s="7">
         <f xml:space="preserve"> (C4+D4) / B4</f>
-        <v>0.1875</v>
+        <v>0.23529411764705882</v>
       </c>
       <c r="I4" s="7">
         <f xml:space="preserve"> B4 / Game_Record!$H$2</f>
-        <v>0.8</v>
+        <v>0.80952380952380953</v>
       </c>
       <c r="J4" s="10">
         <f xml:space="preserve"> K4/B4</f>
-        <v>1</v>
+        <v>1.1176470588235294</v>
       </c>
       <c r="K4" s="2">
         <f xml:space="preserve"> (C4 * 5) + (D4 * 3) + (E4 * 1)</f>
-        <v>16</v>
+        <v>19</v>
       </c>
     </row>
     <row r="5" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
@@ -1267,7 +1294,7 @@
       </c>
       <c r="I5" s="7">
         <f xml:space="preserve"> B5 / Game_Record!$H$2</f>
-        <v>0.9</v>
+        <v>0.8571428571428571</v>
       </c>
       <c r="J5" s="10">
         <f xml:space="preserve"> K5/B5</f>
@@ -1284,11 +1311,11 @@
       </c>
       <c r="B6" s="2">
         <f xml:space="preserve"> C6 + D6 + E6 + F6</f>
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C6" s="2">
         <f>COUNTIF(Game_Record!C2:C101, "SimpleJack")</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D6" s="2">
         <f>COUNTIF(Game_Record!D2:D101, "SimpleJack")</f>
@@ -1304,23 +1331,23 @@
       </c>
       <c r="G6" s="3">
         <f xml:space="preserve"> C6 / B6</f>
-        <v>0</v>
+        <v>0.05</v>
       </c>
       <c r="H6" s="7">
         <f xml:space="preserve"> (C6+D6) / B6</f>
-        <v>0.10526315789473684</v>
+        <v>0.15</v>
       </c>
       <c r="I6" s="7">
         <f xml:space="preserve"> B6 / Game_Record!$H$2</f>
-        <v>0.95</v>
+        <v>0.95238095238095233</v>
       </c>
       <c r="J6" s="10">
         <f xml:space="preserve"> K6/B6</f>
-        <v>0.63157894736842102</v>
+        <v>0.85</v>
       </c>
       <c r="K6" s="2">
         <f xml:space="preserve"> (C6 * 5) + (D6 * 3) + (E6 * 1)</f>
-        <v>12</v>
+        <v>17</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Wed Feb 11 00:30:54 EST 2026
</commit_message>
<xml_diff>
--- a/Doont.xlsx
+++ b/Doont.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cmatt\OneDrive\doont\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44F2C5FC-C40F-4254-B948-D47E3F0FB446}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{586DC36E-6749-40DA-B243-B3C36DFCEDC4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4365" yWindow="1110" windowWidth="23550" windowHeight="11880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2925" yWindow="930" windowWidth="23550" windowHeight="11880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Game_Record" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="26">
   <si>
     <t>Game #</t>
   </si>
@@ -112,6 +112,9 @@
   </si>
   <si>
     <t>End</t>
+  </si>
+  <si>
+    <t>Duration</t>
   </si>
 </sst>
 </file>
@@ -554,10 +557,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J22"/>
+  <dimension ref="A1:K23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A23" sqref="A23"/>
+    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="K21" sqref="K21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -572,10 +575,11 @@
     <col min="8" max="8" width="25.5703125" style="5" customWidth="1"/>
     <col min="9" max="9" width="13.5703125" style="5" customWidth="1"/>
     <col min="10" max="10" width="12.85546875" style="5" customWidth="1"/>
-    <col min="11" max="16384" width="9.140625" style="5"/>
+    <col min="11" max="11" width="13" style="5" customWidth="1"/>
+    <col min="12" max="16384" width="9.140625" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" ht="37.5" x14ac:dyDescent="0.25">
       <c r="A1" s="14" t="s">
         <v>0</v>
       </c>
@@ -604,8 +608,11 @@
       <c r="J1" s="14" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="2" spans="1:10" ht="21" x14ac:dyDescent="0.25">
+      <c r="K1" s="14" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" ht="21" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
         <f>ROW()-1</f>
         <v>1</v>
@@ -627,10 +634,10 @@
       </c>
       <c r="H2" s="17">
         <f>COUNTA(Game_Record!B2:B101)</f>
-        <v>21</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
         <f t="shared" ref="A3:A7" si="0">ROW()-1</f>
         <v>2</v>
@@ -651,7 +658,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
         <f t="shared" si="0"/>
         <v>3</v>
@@ -672,7 +679,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
         <f t="shared" si="0"/>
         <v>4</v>
@@ -693,7 +700,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
         <f t="shared" si="0"/>
         <v>5</v>
@@ -714,7 +721,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
         <f t="shared" si="0"/>
         <v>6</v>
@@ -735,9 +742,9 @@
         <v>18</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" s="5">
-        <f t="shared" ref="A8:A22" si="1">ROW()-1</f>
+        <f t="shared" ref="A8:A23" si="1">ROW()-1</f>
         <v>7</v>
       </c>
       <c r="B8" s="6">
@@ -756,7 +763,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" s="5">
         <f t="shared" si="1"/>
         <v>8</v>
@@ -777,7 +784,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" s="5">
         <f t="shared" si="1"/>
         <v>9</v>
@@ -798,7 +805,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" s="5">
         <f t="shared" si="1"/>
         <v>10</v>
@@ -819,7 +826,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" s="5">
         <f t="shared" si="1"/>
         <v>11</v>
@@ -840,7 +847,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" s="5">
         <f t="shared" si="1"/>
         <v>12</v>
@@ -861,7 +868,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" s="5">
         <f t="shared" si="1"/>
         <v>13</v>
@@ -882,7 +889,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" s="5">
         <f t="shared" si="1"/>
         <v>14</v>
@@ -903,7 +910,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" s="5">
         <f t="shared" si="1"/>
         <v>15</v>
@@ -924,7 +931,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17" s="5">
         <f t="shared" si="1"/>
         <v>16</v>
@@ -945,7 +952,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" s="5">
         <f t="shared" si="1"/>
         <v>17</v>
@@ -966,7 +973,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" s="5">
         <f t="shared" si="1"/>
         <v>18</v>
@@ -987,7 +994,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20" s="5">
         <f t="shared" si="1"/>
         <v>19</v>
@@ -1008,7 +1015,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21" s="5">
         <f t="shared" si="1"/>
         <v>20</v>
@@ -1034,8 +1041,12 @@
       <c r="J21" s="18">
         <v>0.9458333333333333</v>
       </c>
-    </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K21" s="18">
+        <f>MOD(J21 - I21, 1)</f>
+        <v>7.3611111111111072E-2</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A22" s="5">
         <f t="shared" si="1"/>
         <v>21</v>
@@ -1061,9 +1072,45 @@
       <c r="J22" s="18">
         <v>0.95763888888888893</v>
       </c>
+      <c r="K22" s="18">
+        <f>MOD(J22 - I22, 1)</f>
+        <v>7.986111111111116E-2</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A23" s="5">
+        <f t="shared" si="1"/>
+        <v>22</v>
+      </c>
+      <c r="B23" s="6">
+        <v>46063</v>
+      </c>
+      <c r="C23" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="D23" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="E23" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="F23" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="I23" s="18">
+        <v>0.86736111111111114</v>
+      </c>
+      <c r="J23" s="18">
+        <v>0.92291666666666672</v>
+      </c>
+      <c r="K23" s="18">
+        <f>MOD(J23 - I23, 1)</f>
+        <v>5.555555555555558E-2</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1072,7 +1119,7 @@
   <dimension ref="A1:K9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K7" sqref="K7"/>
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1131,7 +1178,7 @@
       </c>
       <c r="B2" s="2">
         <f xml:space="preserve"> C2 + D2 + E2 + F2</f>
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C2" s="2">
         <f>COUNTIF(Game_Record!C2:C101, "Doanage")</f>
@@ -1139,7 +1186,7 @@
       </c>
       <c r="D2" s="2">
         <f>COUNTIF(Game_Record!D2:D101, "Doanage")</f>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E2" s="2">
         <f>COUNTIF(Game_Record!E2:E101, "Doanage")</f>
@@ -1151,23 +1198,23 @@
       </c>
       <c r="G2" s="3">
         <f xml:space="preserve"> C2 / B2</f>
-        <v>0.53333333333333333</v>
+        <v>0.5</v>
       </c>
       <c r="H2" s="7">
         <f xml:space="preserve"> (C2+D2) / B2</f>
-        <v>0.73333333333333328</v>
+        <v>0.75</v>
       </c>
       <c r="I2" s="7">
         <f xml:space="preserve"> B2 / Game_Record!$H$2</f>
-        <v>0.7142857142857143</v>
+        <v>0.72727272727272729</v>
       </c>
       <c r="J2" s="10">
         <f xml:space="preserve"> K2/B2</f>
-        <v>3.4666666666666668</v>
+        <v>3.4375</v>
       </c>
       <c r="K2" s="2">
         <f xml:space="preserve"> (C2 * 5) + (D2 * 3) + (E2 * 1)</f>
-        <v>52</v>
+        <v>55</v>
       </c>
     </row>
     <row r="3" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
@@ -1204,7 +1251,7 @@
       </c>
       <c r="I3" s="7">
         <f xml:space="preserve"> B3 / Game_Record!$H$2</f>
-        <v>0.66666666666666663</v>
+        <v>0.63636363636363635</v>
       </c>
       <c r="J3" s="10">
         <f xml:space="preserve"> K3/B3</f>
@@ -1221,7 +1268,7 @@
       </c>
       <c r="B4" s="2">
         <f xml:space="preserve"> C4 + D4 + E4 + F4</f>
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C4" s="2">
         <f>COUNTIF(Game_Record!C2:C101, "DrSystomatix")</f>
@@ -1233,7 +1280,7 @@
       </c>
       <c r="E4" s="2">
         <f>COUNTIF(Game_Record!E2:E101, "DrSystomatix")</f>
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="F4" s="2">
         <f>COUNTIF(Game_Record!F2:F101, "DrSystomatix")</f>
@@ -1245,19 +1292,19 @@
       </c>
       <c r="H4" s="7">
         <f xml:space="preserve"> (C4+D4) / B4</f>
-        <v>0.23529411764705882</v>
+        <v>0.22222222222222221</v>
       </c>
       <c r="I4" s="7">
         <f xml:space="preserve"> B4 / Game_Record!$H$2</f>
-        <v>0.80952380952380953</v>
+        <v>0.81818181818181823</v>
       </c>
       <c r="J4" s="10">
         <f xml:space="preserve"> K4/B4</f>
-        <v>1.1176470588235294</v>
+        <v>1.1111111111111112</v>
       </c>
       <c r="K4" s="2">
         <f xml:space="preserve"> (C4 * 5) + (D4 * 3) + (E4 * 1)</f>
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="5" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
@@ -1266,11 +1313,11 @@
       </c>
       <c r="B5" s="2">
         <f xml:space="preserve"> C5 + D5 + E5 + F5</f>
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C5" s="2">
         <f>COUNTIF(Game_Record!C2:C101, "Player1")</f>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D5" s="2">
         <f>COUNTIF(Game_Record!D2:D101, "Player1")</f>
@@ -1286,23 +1333,23 @@
       </c>
       <c r="G5" s="3">
         <f xml:space="preserve"> C5 / B5</f>
-        <v>0.22222222222222221</v>
+        <v>0.26315789473684209</v>
       </c>
       <c r="H5" s="7">
         <f xml:space="preserve"> (C5+D5) / B5</f>
-        <v>0.61111111111111116</v>
+        <v>0.63157894736842102</v>
       </c>
       <c r="I5" s="7">
         <f xml:space="preserve"> B5 / Game_Record!$H$2</f>
-        <v>0.8571428571428571</v>
+        <v>0.86363636363636365</v>
       </c>
       <c r="J5" s="10">
         <f xml:space="preserve"> K5/B5</f>
-        <v>2.5555555555555554</v>
+        <v>2.6842105263157894</v>
       </c>
       <c r="K5" s="2">
         <f xml:space="preserve"> (C5 * 5) + (D5 * 3) + (E5 * 1)</f>
-        <v>46</v>
+        <v>51</v>
       </c>
     </row>
     <row r="6" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
@@ -1311,7 +1358,7 @@
       </c>
       <c r="B6" s="2">
         <f xml:space="preserve"> C6 + D6 + E6 + F6</f>
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C6" s="2">
         <f>COUNTIF(Game_Record!C2:C101, "SimpleJack")</f>
@@ -1327,23 +1374,23 @@
       </c>
       <c r="F6" s="2">
         <f>COUNTIF(Game_Record!F2:F101, "SimpleJack")</f>
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G6" s="3">
         <f xml:space="preserve"> C6 / B6</f>
-        <v>0.05</v>
+        <v>4.7619047619047616E-2</v>
       </c>
       <c r="H6" s="7">
         <f xml:space="preserve"> (C6+D6) / B6</f>
-        <v>0.15</v>
+        <v>0.14285714285714285</v>
       </c>
       <c r="I6" s="7">
         <f xml:space="preserve"> B6 / Game_Record!$H$2</f>
-        <v>0.95238095238095233</v>
+        <v>0.95454545454545459</v>
       </c>
       <c r="J6" s="10">
         <f xml:space="preserve"> K6/B6</f>
-        <v>0.85</v>
+        <v>0.80952380952380953</v>
       </c>
       <c r="K6" s="2">
         <f xml:space="preserve"> (C6 * 5) + (D6 * 3) + (E6 * 1)</f>

</xml_diff>